<commit_message>
removal of bad data
</commit_message>
<xml_diff>
--- a/FinalProjectGuide.xlsx
+++ b/FinalProjectGuide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Documents\GitHub\FinalProject-MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F600B7-38B5-45C9-A68B-7FA00395DAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5CB91D-0278-40F6-90EA-4DAEA467604C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="18000" windowHeight="9360" firstSheet="7" activeTab="7" xr2:uid="{9D2C2162-F178-4CB0-81E9-DFAA2C429D49}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="7" activeTab="9" xr2:uid="{9D2C2162-F178-4CB0-81E9-DFAA2C429D49}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="511">
   <si>
     <t>Python Pandas</t>
   </si>
@@ -1425,6 +1425,156 @@
   </si>
   <si>
     <t>https://github.com/jlugomar/longitudinal_microbiome_analysis_public/tree/master/datasets</t>
+  </si>
+  <si>
+    <t>SubjectID</t>
+  </si>
+  <si>
+    <t>Day of life sample obtained</t>
+  </si>
+  <si>
+    <t>Gestational age at birth</t>
+  </si>
+  <si>
+    <t>Postconceptional age sample obtained</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Mode of birth</t>
+  </si>
+  <si>
+    <t>Room type</t>
+  </si>
+  <si>
+    <t>Human milk used</t>
+  </si>
+  <si>
+    <t>Days of antibiotics</t>
+  </si>
+  <si>
+    <t>Actinobacteria</t>
+  </si>
+  <si>
+    <t>Alphaproteobacteria</t>
+  </si>
+  <si>
+    <t>Bacilli</t>
+  </si>
+  <si>
+    <t>Bacteroidia</t>
+  </si>
+  <si>
+    <t>Betaproteobacteria</t>
+  </si>
+  <si>
+    <t>Clostridia</t>
+  </si>
+  <si>
+    <t>Cyanobacteria</t>
+  </si>
+  <si>
+    <t>Epsilonproteobacteria</t>
+  </si>
+  <si>
+    <t>Erysipelotrichi</t>
+  </si>
+  <si>
+    <t>Flavobacteria</t>
+  </si>
+  <si>
+    <t>Fusobacteria</t>
+  </si>
+  <si>
+    <t>Gammaproteobacteria</t>
+  </si>
+  <si>
+    <t>Holophagae</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>Day sample obtained</t>
+  </si>
+  <si>
+    <t>Gestational day of delivery</t>
+  </si>
+  <si>
+    <t>Day_Period</t>
+  </si>
+  <si>
+    <t>Aerococcus</t>
+  </si>
+  <si>
+    <t>Anaerococcus</t>
+  </si>
+  <si>
+    <t>Ureaplasma</t>
+  </si>
+  <si>
+    <t>Parvimonas</t>
+  </si>
+  <si>
+    <t>L. iners</t>
+  </si>
+  <si>
+    <t>Finegoldia</t>
+  </si>
+  <si>
+    <t>Staphylococcus</t>
+  </si>
+  <si>
+    <t>Porphyromonas</t>
+  </si>
+  <si>
+    <t>Atopobium</t>
+  </si>
+  <si>
+    <t>Gardnerella</t>
+  </si>
+  <si>
+    <t>L. crispatus</t>
+  </si>
+  <si>
+    <t>Peptostreptococcus</t>
+  </si>
+  <si>
+    <t>Sneathia</t>
+  </si>
+  <si>
+    <t>Streptococcus</t>
+  </si>
+  <si>
+    <t>Prevotella</t>
+  </si>
+  <si>
+    <t>Peptoniphilus</t>
+  </si>
+  <si>
+    <t>Incertae_Sedis_XI.1</t>
+  </si>
+  <si>
+    <t>L. gasseri</t>
+  </si>
+  <si>
+    <t>Corynebacterium</t>
+  </si>
+  <si>
+    <t>Dialister</t>
+  </si>
+  <si>
+    <t>L.otu5</t>
+  </si>
+  <si>
+    <t>L.otu3</t>
+  </si>
+  <si>
+    <t>Ruminococcaceae.3</t>
+  </si>
+  <si>
+    <t>https://github.com/jlugomar/longitudinal_microbiome_analysis_public</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1585,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1596,8 +1746,20 @@
       <color rgb="FF1D1C1D"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1652,8 +1814,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1805,6 +1973,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1813,7 +2009,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1964,15 +2160,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1991,6 +2180,28 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="26" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="26" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2909,13 +3120,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CC48AC-513D-4AB1-BAEC-B7050A391FC0}">
-  <dimension ref="A1:RU78"/>
+  <dimension ref="A1:RU100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:489" ht="27.75">
       <c r="A1" s="18" t="s">
@@ -2930,76 +3144,76 @@
       <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:489" ht="15.75" thickBot="1">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="F3" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="66" t="s">
+      <c r="H3" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="66" t="s">
+      <c r="I3" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="66" t="s">
+      <c r="J3" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="64" t="s">
+      <c r="K3" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="66" t="s">
+      <c r="P3" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="Q3" s="66" t="s">
+      <c r="Q3" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="66" t="s">
+      <c r="R3" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="S3" s="66" t="s">
+      <c r="S3" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="66" t="s">
+      <c r="T3" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="U3" s="64" t="s">
+      <c r="U3" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
+      <c r="V3" s="62"/>
+      <c r="W3" s="62"/>
+      <c r="X3" s="62"/>
     </row>
     <row r="4" spans="1:489" ht="30.95" customHeight="1" thickBot="1">
-      <c r="A4" s="69"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
       <c r="K4" s="4" t="s">
         <v>96</v>
       </c>
@@ -3013,11 +3227,11 @@
         <v>99</v>
       </c>
       <c r="O4" s="3"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
       <c r="U4" s="4" t="s">
         <v>96</v>
       </c>
@@ -3129,848 +3343,848 @@
     </row>
     <row r="7" spans="1:489" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:489" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A8" s="70"/>
-      <c r="B8" s="68" t="s">
+      <c r="A8" s="67"/>
+      <c r="B8" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="66" t="s">
+      <c r="D8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="F8" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="H8" s="68" t="s">
+      <c r="H8" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="66" t="s">
+      <c r="I8" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="J8" s="64" t="s">
+      <c r="J8" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64" t="s">
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="64" t="s">
+      <c r="P8" s="62"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="T8" s="64" t="s">
+      <c r="T8" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="64" t="s">
+      <c r="U8" s="62"/>
+      <c r="V8" s="62"/>
+      <c r="W8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="X8" s="64"/>
-      <c r="Y8" s="64" t="s">
+      <c r="X8" s="62"/>
+      <c r="Y8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="Z8" s="64"/>
-      <c r="AA8" s="64" t="s">
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="AB8" s="64"/>
-      <c r="AC8" s="64"/>
-      <c r="AD8" s="64" t="s">
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="62"/>
+      <c r="AD8" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="AE8" s="64" t="s">
+      <c r="AE8" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="AF8" s="64"/>
-      <c r="AG8" s="64"/>
-      <c r="AH8" s="64"/>
-      <c r="AI8" s="64" t="s">
+      <c r="AF8" s="62"/>
+      <c r="AG8" s="62"/>
+      <c r="AH8" s="62"/>
+      <c r="AI8" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="AJ8" s="64"/>
-      <c r="AK8" s="64" t="s">
+      <c r="AJ8" s="62"/>
+      <c r="AK8" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="AL8" s="64"/>
-      <c r="AM8" s="64"/>
-      <c r="AN8" s="64" t="s">
+      <c r="AL8" s="62"/>
+      <c r="AM8" s="62"/>
+      <c r="AN8" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="AO8" s="64" t="s">
+      <c r="AO8" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="AP8" s="64"/>
-      <c r="AQ8" s="64"/>
-      <c r="AR8" s="64"/>
-      <c r="AS8" s="64" t="s">
+      <c r="AP8" s="62"/>
+      <c r="AQ8" s="62"/>
+      <c r="AR8" s="62"/>
+      <c r="AS8" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="AT8" s="64"/>
-      <c r="AU8" s="64"/>
-      <c r="AV8" s="64"/>
-      <c r="AW8" s="64"/>
-      <c r="AX8" s="64" t="s">
+      <c r="AT8" s="62"/>
+      <c r="AU8" s="62"/>
+      <c r="AV8" s="62"/>
+      <c r="AW8" s="62"/>
+      <c r="AX8" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="AY8" s="64"/>
-      <c r="AZ8" s="64"/>
-      <c r="BA8" s="64"/>
-      <c r="BB8" s="64" t="s">
+      <c r="AY8" s="62"/>
+      <c r="AZ8" s="62"/>
+      <c r="BA8" s="62"/>
+      <c r="BB8" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="BC8" s="64" t="s">
+      <c r="BC8" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="BD8" s="64"/>
-      <c r="BE8" s="64"/>
-      <c r="BF8" s="64" t="s">
+      <c r="BD8" s="62"/>
+      <c r="BE8" s="62"/>
+      <c r="BF8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="BG8" s="64"/>
-      <c r="BH8" s="64" t="s">
+      <c r="BG8" s="62"/>
+      <c r="BH8" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="BI8" s="64"/>
-      <c r="BJ8" s="64" t="s">
+      <c r="BI8" s="62"/>
+      <c r="BJ8" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="BK8" s="64"/>
-      <c r="BL8" s="64"/>
-      <c r="BM8" s="64" t="s">
+      <c r="BK8" s="62"/>
+      <c r="BL8" s="62"/>
+      <c r="BM8" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="BN8" s="64" t="s">
+      <c r="BN8" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="BO8" s="64"/>
-      <c r="BP8" s="64"/>
-      <c r="BQ8" s="64"/>
-      <c r="BR8" s="64" t="s">
+      <c r="BO8" s="62"/>
+      <c r="BP8" s="62"/>
+      <c r="BQ8" s="62"/>
+      <c r="BR8" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="BS8" s="64"/>
-      <c r="BT8" s="64"/>
-      <c r="BU8" s="64"/>
-      <c r="BV8" s="64"/>
-      <c r="BW8" s="64" t="s">
+      <c r="BS8" s="62"/>
+      <c r="BT8" s="62"/>
+      <c r="BU8" s="62"/>
+      <c r="BV8" s="62"/>
+      <c r="BW8" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="BX8" s="64"/>
-      <c r="BY8" s="64"/>
-      <c r="BZ8" s="64"/>
-      <c r="CA8" s="64" t="s">
+      <c r="BX8" s="62"/>
+      <c r="BY8" s="62"/>
+      <c r="BZ8" s="62"/>
+      <c r="CA8" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="CB8" s="64" t="s">
+      <c r="CB8" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="CC8" s="64"/>
-      <c r="CD8" s="64"/>
-      <c r="CE8" s="64" t="s">
+      <c r="CC8" s="62"/>
+      <c r="CD8" s="62"/>
+      <c r="CE8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="CF8" s="64"/>
-      <c r="CG8" s="64" t="s">
+      <c r="CF8" s="62"/>
+      <c r="CG8" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="CH8" s="64"/>
-      <c r="CI8" s="64" t="s">
+      <c r="CH8" s="62"/>
+      <c r="CI8" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="CJ8" s="64"/>
-      <c r="CK8" s="64"/>
-      <c r="CL8" s="64" t="s">
+      <c r="CJ8" s="62"/>
+      <c r="CK8" s="62"/>
+      <c r="CL8" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="CM8" s="64" t="s">
+      <c r="CM8" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="CN8" s="64"/>
-      <c r="CO8" s="64"/>
-      <c r="CP8" s="64"/>
-      <c r="CQ8" s="64" t="s">
+      <c r="CN8" s="62"/>
+      <c r="CO8" s="62"/>
+      <c r="CP8" s="62"/>
+      <c r="CQ8" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="CR8" s="64"/>
-      <c r="CS8" s="64"/>
-      <c r="CT8" s="64"/>
-      <c r="CU8" s="64"/>
-      <c r="CV8" s="64" t="s">
+      <c r="CR8" s="62"/>
+      <c r="CS8" s="62"/>
+      <c r="CT8" s="62"/>
+      <c r="CU8" s="62"/>
+      <c r="CV8" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="CW8" s="64"/>
-      <c r="CX8" s="64"/>
-      <c r="CY8" s="64"/>
-      <c r="CZ8" s="64" t="s">
+      <c r="CW8" s="62"/>
+      <c r="CX8" s="62"/>
+      <c r="CY8" s="62"/>
+      <c r="CZ8" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="DA8" s="64" t="s">
+      <c r="DA8" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="DB8" s="64"/>
-      <c r="DC8" s="64"/>
-      <c r="DD8" s="64" t="s">
+      <c r="DB8" s="62"/>
+      <c r="DC8" s="62"/>
+      <c r="DD8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="DE8" s="64"/>
-      <c r="DF8" s="64" t="s">
+      <c r="DE8" s="62"/>
+      <c r="DF8" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="DG8" s="64"/>
-      <c r="DH8" s="64" t="s">
+      <c r="DG8" s="62"/>
+      <c r="DH8" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="DI8" s="64"/>
-      <c r="DJ8" s="64"/>
-      <c r="DK8" s="64" t="s">
+      <c r="DI8" s="62"/>
+      <c r="DJ8" s="62"/>
+      <c r="DK8" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="DL8" s="64" t="s">
+      <c r="DL8" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="DM8" s="64"/>
-      <c r="DN8" s="64"/>
-      <c r="DO8" s="64"/>
-      <c r="DP8" s="64" t="s">
+      <c r="DM8" s="62"/>
+      <c r="DN8" s="62"/>
+      <c r="DO8" s="62"/>
+      <c r="DP8" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="DQ8" s="64"/>
-      <c r="DR8" s="64"/>
-      <c r="DS8" s="64"/>
-      <c r="DT8" s="64"/>
-      <c r="DU8" s="64" t="s">
+      <c r="DQ8" s="62"/>
+      <c r="DR8" s="62"/>
+      <c r="DS8" s="62"/>
+      <c r="DT8" s="62"/>
+      <c r="DU8" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="DV8" s="64"/>
-      <c r="DW8" s="64"/>
-      <c r="DX8" s="64"/>
-      <c r="DY8" s="64" t="s">
+      <c r="DV8" s="62"/>
+      <c r="DW8" s="62"/>
+      <c r="DX8" s="62"/>
+      <c r="DY8" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="DZ8" s="64" t="s">
+      <c r="DZ8" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="EA8" s="64"/>
-      <c r="EB8" s="64"/>
-      <c r="EC8" s="64" t="s">
+      <c r="EA8" s="62"/>
+      <c r="EB8" s="62"/>
+      <c r="EC8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="ED8" s="64"/>
-      <c r="EE8" s="64"/>
-      <c r="EF8" s="64" t="s">
+      <c r="ED8" s="62"/>
+      <c r="EE8" s="62"/>
+      <c r="EF8" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="EG8" s="64"/>
-      <c r="EH8" s="64"/>
-      <c r="EI8" s="64" t="s">
+      <c r="EG8" s="62"/>
+      <c r="EH8" s="62"/>
+      <c r="EI8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="EJ8" s="64"/>
-      <c r="EK8" s="64"/>
-      <c r="EL8" s="64" t="s">
+      <c r="EJ8" s="62"/>
+      <c r="EK8" s="62"/>
+      <c r="EL8" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="EM8" s="64"/>
-      <c r="EN8" s="64"/>
-      <c r="EO8" s="64" t="s">
+      <c r="EM8" s="62"/>
+      <c r="EN8" s="62"/>
+      <c r="EO8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="EP8" s="64"/>
-      <c r="EQ8" s="64"/>
-      <c r="ER8" s="64" t="s">
+      <c r="EP8" s="62"/>
+      <c r="EQ8" s="62"/>
+      <c r="ER8" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="ES8" s="64"/>
-      <c r="ET8" s="64"/>
-      <c r="EU8" s="64" t="s">
+      <c r="ES8" s="62"/>
+      <c r="ET8" s="62"/>
+      <c r="EU8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="EV8" s="64"/>
-      <c r="EW8" s="64"/>
-      <c r="EX8" s="64" t="s">
+      <c r="EV8" s="62"/>
+      <c r="EW8" s="62"/>
+      <c r="EX8" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="EY8" s="64"/>
-      <c r="EZ8" s="64"/>
-      <c r="FA8" s="64" t="s">
+      <c r="EY8" s="62"/>
+      <c r="EZ8" s="62"/>
+      <c r="FA8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="FB8" s="64"/>
-      <c r="FC8" s="64"/>
-      <c r="FD8" s="64" t="s">
+      <c r="FB8" s="62"/>
+      <c r="FC8" s="62"/>
+      <c r="FD8" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="FE8" s="64"/>
-      <c r="FF8" s="64"/>
-      <c r="FG8" s="64" t="s">
+      <c r="FE8" s="62"/>
+      <c r="FF8" s="62"/>
+      <c r="FG8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="FH8" s="64"/>
-      <c r="FI8" s="64"/>
-      <c r="FJ8" s="64" t="s">
+      <c r="FH8" s="62"/>
+      <c r="FI8" s="62"/>
+      <c r="FJ8" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="FK8" s="64"/>
-      <c r="FL8" s="64"/>
-      <c r="FM8" s="64" t="s">
+      <c r="FK8" s="62"/>
+      <c r="FL8" s="62"/>
+      <c r="FM8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="FN8" s="64"/>
-      <c r="FO8" s="64"/>
-      <c r="FP8" s="64" t="s">
+      <c r="FN8" s="62"/>
+      <c r="FO8" s="62"/>
+      <c r="FP8" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="FQ8" s="64"/>
-      <c r="FR8" s="64"/>
-      <c r="FS8" s="64" t="s">
+      <c r="FQ8" s="62"/>
+      <c r="FR8" s="62"/>
+      <c r="FS8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="FT8" s="64"/>
-      <c r="FU8" s="64"/>
-      <c r="FV8" s="64" t="s">
+      <c r="FT8" s="62"/>
+      <c r="FU8" s="62"/>
+      <c r="FV8" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="FW8" s="64"/>
-      <c r="FX8" s="64"/>
-      <c r="FY8" s="64" t="s">
+      <c r="FW8" s="62"/>
+      <c r="FX8" s="62"/>
+      <c r="FY8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="FZ8" s="64"/>
-      <c r="GA8" s="64"/>
-      <c r="GB8" s="64" t="s">
+      <c r="FZ8" s="62"/>
+      <c r="GA8" s="62"/>
+      <c r="GB8" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="GC8" s="64"/>
-      <c r="GD8" s="64"/>
-      <c r="GE8" s="64" t="s">
+      <c r="GC8" s="62"/>
+      <c r="GD8" s="62"/>
+      <c r="GE8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="GF8" s="64"/>
-      <c r="GG8" s="64"/>
-      <c r="GH8" s="64" t="s">
+      <c r="GF8" s="62"/>
+      <c r="GG8" s="62"/>
+      <c r="GH8" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="GI8" s="64"/>
-      <c r="GJ8" s="64"/>
-      <c r="GK8" s="64" t="s">
+      <c r="GI8" s="62"/>
+      <c r="GJ8" s="62"/>
+      <c r="GK8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="GL8" s="64"/>
-      <c r="GM8" s="64"/>
-      <c r="GN8" s="64" t="s">
+      <c r="GL8" s="62"/>
+      <c r="GM8" s="62"/>
+      <c r="GN8" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="GO8" s="64"/>
-      <c r="GP8" s="64"/>
-      <c r="GQ8" s="64" t="s">
+      <c r="GO8" s="62"/>
+      <c r="GP8" s="62"/>
+      <c r="GQ8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="GR8" s="64"/>
-      <c r="GS8" s="64"/>
-      <c r="GT8" s="64" t="s">
+      <c r="GR8" s="62"/>
+      <c r="GS8" s="62"/>
+      <c r="GT8" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="GU8" s="64"/>
-      <c r="GV8" s="64"/>
-      <c r="GW8" s="64" t="s">
+      <c r="GU8" s="62"/>
+      <c r="GV8" s="62"/>
+      <c r="GW8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="GX8" s="64"/>
-      <c r="GY8" s="64"/>
-      <c r="GZ8" s="64" t="s">
+      <c r="GX8" s="62"/>
+      <c r="GY8" s="62"/>
+      <c r="GZ8" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="HA8" s="64"/>
-      <c r="HB8" s="64"/>
-      <c r="HC8" s="64" t="s">
+      <c r="HA8" s="62"/>
+      <c r="HB8" s="62"/>
+      <c r="HC8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="HD8" s="64"/>
-      <c r="HE8" s="64"/>
-      <c r="HF8" s="64" t="s">
+      <c r="HD8" s="62"/>
+      <c r="HE8" s="62"/>
+      <c r="HF8" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="HG8" s="64"/>
-      <c r="HH8" s="64"/>
-      <c r="HI8" s="64" t="s">
+      <c r="HG8" s="62"/>
+      <c r="HH8" s="62"/>
+      <c r="HI8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="HJ8" s="64"/>
-      <c r="HK8" s="64"/>
-      <c r="HL8" s="64" t="s">
+      <c r="HJ8" s="62"/>
+      <c r="HK8" s="62"/>
+      <c r="HL8" s="62" t="s">
         <v>150</v>
       </c>
-      <c r="HM8" s="64"/>
-      <c r="HN8" s="64"/>
-      <c r="HO8" s="64" t="s">
+      <c r="HM8" s="62"/>
+      <c r="HN8" s="62"/>
+      <c r="HO8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="HP8" s="64"/>
-      <c r="HQ8" s="64"/>
-      <c r="HR8" s="64" t="s">
+      <c r="HP8" s="62"/>
+      <c r="HQ8" s="62"/>
+      <c r="HR8" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="HS8" s="64"/>
-      <c r="HT8" s="64"/>
-      <c r="HU8" s="64" t="s">
+      <c r="HS8" s="62"/>
+      <c r="HT8" s="62"/>
+      <c r="HU8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="HV8" s="64"/>
-      <c r="HW8" s="64"/>
-      <c r="HX8" s="64" t="s">
+      <c r="HV8" s="62"/>
+      <c r="HW8" s="62"/>
+      <c r="HX8" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="HY8" s="64"/>
-      <c r="HZ8" s="64"/>
-      <c r="IA8" s="64" t="s">
+      <c r="HY8" s="62"/>
+      <c r="HZ8" s="62"/>
+      <c r="IA8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="IB8" s="64"/>
-      <c r="IC8" s="64"/>
-      <c r="ID8" s="64" t="s">
+      <c r="IB8" s="62"/>
+      <c r="IC8" s="62"/>
+      <c r="ID8" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="IE8" s="64"/>
-      <c r="IF8" s="64"/>
-      <c r="IG8" s="64" t="s">
+      <c r="IE8" s="62"/>
+      <c r="IF8" s="62"/>
+      <c r="IG8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="IH8" s="64"/>
-      <c r="II8" s="64"/>
-      <c r="IJ8" s="64" t="s">
+      <c r="IH8" s="62"/>
+      <c r="II8" s="62"/>
+      <c r="IJ8" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="IK8" s="64"/>
-      <c r="IL8" s="64"/>
-      <c r="IM8" s="64" t="s">
+      <c r="IK8" s="62"/>
+      <c r="IL8" s="62"/>
+      <c r="IM8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="IN8" s="64"/>
-      <c r="IO8" s="64"/>
-      <c r="IP8" s="64" t="s">
+      <c r="IN8" s="62"/>
+      <c r="IO8" s="62"/>
+      <c r="IP8" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="IQ8" s="64"/>
-      <c r="IR8" s="64"/>
-      <c r="IS8" s="64" t="s">
+      <c r="IQ8" s="62"/>
+      <c r="IR8" s="62"/>
+      <c r="IS8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="IT8" s="64"/>
-      <c r="IU8" s="64"/>
-      <c r="IV8" s="64" t="s">
+      <c r="IT8" s="62"/>
+      <c r="IU8" s="62"/>
+      <c r="IV8" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="IW8" s="64"/>
-      <c r="IX8" s="64"/>
-      <c r="IY8" s="64" t="s">
+      <c r="IW8" s="62"/>
+      <c r="IX8" s="62"/>
+      <c r="IY8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="IZ8" s="64"/>
-      <c r="JA8" s="64"/>
-      <c r="JB8" s="64" t="s">
+      <c r="IZ8" s="62"/>
+      <c r="JA8" s="62"/>
+      <c r="JB8" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="JC8" s="64"/>
-      <c r="JD8" s="64"/>
-      <c r="JE8" s="64" t="s">
+      <c r="JC8" s="62"/>
+      <c r="JD8" s="62"/>
+      <c r="JE8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="JF8" s="64"/>
-      <c r="JG8" s="64"/>
-      <c r="JH8" s="64" t="s">
+      <c r="JF8" s="62"/>
+      <c r="JG8" s="62"/>
+      <c r="JH8" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="JI8" s="64"/>
-      <c r="JJ8" s="64"/>
-      <c r="JK8" s="64" t="s">
+      <c r="JI8" s="62"/>
+      <c r="JJ8" s="62"/>
+      <c r="JK8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="JL8" s="64"/>
-      <c r="JM8" s="64"/>
-      <c r="JN8" s="64" t="s">
+      <c r="JL8" s="62"/>
+      <c r="JM8" s="62"/>
+      <c r="JN8" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="JO8" s="64"/>
-      <c r="JP8" s="64"/>
-      <c r="JQ8" s="64" t="s">
+      <c r="JO8" s="62"/>
+      <c r="JP8" s="62"/>
+      <c r="JQ8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="JR8" s="64"/>
-      <c r="JS8" s="64"/>
-      <c r="JT8" s="64" t="s">
+      <c r="JR8" s="62"/>
+      <c r="JS8" s="62"/>
+      <c r="JT8" s="62" t="s">
         <v>160</v>
       </c>
-      <c r="JU8" s="64"/>
-      <c r="JV8" s="64"/>
-      <c r="JW8" s="64" t="s">
+      <c r="JU8" s="62"/>
+      <c r="JV8" s="62"/>
+      <c r="JW8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="JX8" s="64"/>
-      <c r="JY8" s="64"/>
-      <c r="JZ8" s="64" t="s">
+      <c r="JX8" s="62"/>
+      <c r="JY8" s="62"/>
+      <c r="JZ8" s="62" t="s">
         <v>161</v>
       </c>
-      <c r="KA8" s="64"/>
-      <c r="KB8" s="64"/>
-      <c r="KC8" s="64" t="s">
+      <c r="KA8" s="62"/>
+      <c r="KB8" s="62"/>
+      <c r="KC8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="KD8" s="64"/>
-      <c r="KE8" s="64"/>
-      <c r="KF8" s="64" t="s">
+      <c r="KD8" s="62"/>
+      <c r="KE8" s="62"/>
+      <c r="KF8" s="62" t="s">
         <v>162</v>
       </c>
-      <c r="KG8" s="64"/>
-      <c r="KH8" s="64"/>
-      <c r="KI8" s="64" t="s">
+      <c r="KG8" s="62"/>
+      <c r="KH8" s="62"/>
+      <c r="KI8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="KJ8" s="64"/>
-      <c r="KK8" s="64"/>
-      <c r="KL8" s="64" t="s">
+      <c r="KJ8" s="62"/>
+      <c r="KK8" s="62"/>
+      <c r="KL8" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="KM8" s="64"/>
-      <c r="KN8" s="64"/>
-      <c r="KO8" s="64" t="s">
+      <c r="KM8" s="62"/>
+      <c r="KN8" s="62"/>
+      <c r="KO8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="KP8" s="64"/>
-      <c r="KQ8" s="64"/>
-      <c r="KR8" s="64" t="s">
+      <c r="KP8" s="62"/>
+      <c r="KQ8" s="62"/>
+      <c r="KR8" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="KS8" s="64"/>
-      <c r="KT8" s="64"/>
-      <c r="KU8" s="64" t="s">
+      <c r="KS8" s="62"/>
+      <c r="KT8" s="62"/>
+      <c r="KU8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="KV8" s="64"/>
-      <c r="KW8" s="64"/>
-      <c r="KX8" s="64" t="s">
+      <c r="KV8" s="62"/>
+      <c r="KW8" s="62"/>
+      <c r="KX8" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="KY8" s="64"/>
-      <c r="KZ8" s="64"/>
-      <c r="LA8" s="64" t="s">
+      <c r="KY8" s="62"/>
+      <c r="KZ8" s="62"/>
+      <c r="LA8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="LB8" s="64"/>
-      <c r="LC8" s="64"/>
-      <c r="LD8" s="64" t="s">
+      <c r="LB8" s="62"/>
+      <c r="LC8" s="62"/>
+      <c r="LD8" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="LE8" s="64"/>
-      <c r="LF8" s="64"/>
-      <c r="LG8" s="64" t="s">
+      <c r="LE8" s="62"/>
+      <c r="LF8" s="62"/>
+      <c r="LG8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="LH8" s="64"/>
-      <c r="LI8" s="64"/>
-      <c r="LJ8" s="64" t="s">
+      <c r="LH8" s="62"/>
+      <c r="LI8" s="62"/>
+      <c r="LJ8" s="62" t="s">
         <v>167</v>
       </c>
-      <c r="LK8" s="64"/>
-      <c r="LL8" s="64"/>
-      <c r="LM8" s="64" t="s">
+      <c r="LK8" s="62"/>
+      <c r="LL8" s="62"/>
+      <c r="LM8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="LN8" s="64"/>
-      <c r="LO8" s="64"/>
-      <c r="LP8" s="64" t="s">
+      <c r="LN8" s="62"/>
+      <c r="LO8" s="62"/>
+      <c r="LP8" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="LQ8" s="64"/>
-      <c r="LR8" s="64"/>
-      <c r="LS8" s="64" t="s">
+      <c r="LQ8" s="62"/>
+      <c r="LR8" s="62"/>
+      <c r="LS8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="LT8" s="64"/>
-      <c r="LU8" s="64"/>
-      <c r="LV8" s="64" t="s">
+      <c r="LT8" s="62"/>
+      <c r="LU8" s="62"/>
+      <c r="LV8" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="LW8" s="64"/>
-      <c r="LX8" s="64"/>
-      <c r="LY8" s="64" t="s">
+      <c r="LW8" s="62"/>
+      <c r="LX8" s="62"/>
+      <c r="LY8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="LZ8" s="64"/>
-      <c r="MA8" s="64"/>
-      <c r="MB8" s="64" t="s">
+      <c r="LZ8" s="62"/>
+      <c r="MA8" s="62"/>
+      <c r="MB8" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="MC8" s="64"/>
-      <c r="MD8" s="64"/>
-      <c r="ME8" s="64" t="s">
+      <c r="MC8" s="62"/>
+      <c r="MD8" s="62"/>
+      <c r="ME8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="MF8" s="64"/>
-      <c r="MG8" s="64"/>
-      <c r="MH8" s="64" t="s">
+      <c r="MF8" s="62"/>
+      <c r="MG8" s="62"/>
+      <c r="MH8" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="MI8" s="64"/>
-      <c r="MJ8" s="64"/>
-      <c r="MK8" s="64" t="s">
+      <c r="MI8" s="62"/>
+      <c r="MJ8" s="62"/>
+      <c r="MK8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="ML8" s="64"/>
-      <c r="MM8" s="64"/>
-      <c r="MN8" s="64" t="s">
+      <c r="ML8" s="62"/>
+      <c r="MM8" s="62"/>
+      <c r="MN8" s="62" t="s">
         <v>172</v>
       </c>
-      <c r="MO8" s="64"/>
-      <c r="MP8" s="64"/>
-      <c r="MQ8" s="64" t="s">
+      <c r="MO8" s="62"/>
+      <c r="MP8" s="62"/>
+      <c r="MQ8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="MR8" s="64"/>
-      <c r="MS8" s="64"/>
-      <c r="MT8" s="64" t="s">
+      <c r="MR8" s="62"/>
+      <c r="MS8" s="62"/>
+      <c r="MT8" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="MU8" s="64"/>
-      <c r="MV8" s="64"/>
-      <c r="MW8" s="64" t="s">
+      <c r="MU8" s="62"/>
+      <c r="MV8" s="62"/>
+      <c r="MW8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="MX8" s="64"/>
-      <c r="MY8" s="64"/>
-      <c r="MZ8" s="64" t="s">
+      <c r="MX8" s="62"/>
+      <c r="MY8" s="62"/>
+      <c r="MZ8" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="NA8" s="64"/>
-      <c r="NB8" s="64"/>
-      <c r="NC8" s="64" t="s">
+      <c r="NA8" s="62"/>
+      <c r="NB8" s="62"/>
+      <c r="NC8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="ND8" s="64"/>
-      <c r="NE8" s="64"/>
-      <c r="NF8" s="64" t="s">
+      <c r="ND8" s="62"/>
+      <c r="NE8" s="62"/>
+      <c r="NF8" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="NG8" s="64"/>
-      <c r="NH8" s="64"/>
-      <c r="NI8" s="64" t="s">
+      <c r="NG8" s="62"/>
+      <c r="NH8" s="62"/>
+      <c r="NI8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="NJ8" s="64"/>
-      <c r="NK8" s="64"/>
-      <c r="NL8" s="64" t="s">
+      <c r="NJ8" s="62"/>
+      <c r="NK8" s="62"/>
+      <c r="NL8" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="NM8" s="64"/>
-      <c r="NN8" s="64"/>
-      <c r="NO8" s="64" t="s">
+      <c r="NM8" s="62"/>
+      <c r="NN8" s="62"/>
+      <c r="NO8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="NP8" s="64"/>
-      <c r="NQ8" s="64"/>
-      <c r="NR8" s="64" t="s">
+      <c r="NP8" s="62"/>
+      <c r="NQ8" s="62"/>
+      <c r="NR8" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="NS8" s="64"/>
-      <c r="NT8" s="64"/>
-      <c r="NU8" s="64" t="s">
+      <c r="NS8" s="62"/>
+      <c r="NT8" s="62"/>
+      <c r="NU8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="NV8" s="64"/>
-      <c r="NW8" s="64"/>
-      <c r="NX8" s="64" t="s">
+      <c r="NV8" s="62"/>
+      <c r="NW8" s="62"/>
+      <c r="NX8" s="62" t="s">
         <v>178</v>
       </c>
-      <c r="NY8" s="64"/>
-      <c r="NZ8" s="64"/>
-      <c r="OA8" s="64" t="s">
+      <c r="NY8" s="62"/>
+      <c r="NZ8" s="62"/>
+      <c r="OA8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="OB8" s="64"/>
-      <c r="OC8" s="64"/>
-      <c r="OD8" s="64" t="s">
+      <c r="OB8" s="62"/>
+      <c r="OC8" s="62"/>
+      <c r="OD8" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="OE8" s="64"/>
-      <c r="OF8" s="64"/>
-      <c r="OG8" s="64" t="s">
+      <c r="OE8" s="62"/>
+      <c r="OF8" s="62"/>
+      <c r="OG8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="OH8" s="64"/>
-      <c r="OI8" s="64"/>
-      <c r="OJ8" s="64" t="s">
+      <c r="OH8" s="62"/>
+      <c r="OI8" s="62"/>
+      <c r="OJ8" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="OK8" s="64"/>
-      <c r="OL8" s="64"/>
-      <c r="OM8" s="64" t="s">
+      <c r="OK8" s="62"/>
+      <c r="OL8" s="62"/>
+      <c r="OM8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="ON8" s="64"/>
-      <c r="OO8" s="64"/>
-      <c r="OP8" s="64" t="s">
+      <c r="ON8" s="62"/>
+      <c r="OO8" s="62"/>
+      <c r="OP8" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="OQ8" s="64"/>
-      <c r="OR8" s="64"/>
-      <c r="OS8" s="64" t="s">
+      <c r="OQ8" s="62"/>
+      <c r="OR8" s="62"/>
+      <c r="OS8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="OT8" s="64"/>
-      <c r="OU8" s="64"/>
-      <c r="OV8" s="64" t="s">
+      <c r="OT8" s="62"/>
+      <c r="OU8" s="62"/>
+      <c r="OV8" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="OW8" s="64"/>
-      <c r="OX8" s="64"/>
-      <c r="OY8" s="64" t="s">
+      <c r="OW8" s="62"/>
+      <c r="OX8" s="62"/>
+      <c r="OY8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="OZ8" s="64"/>
-      <c r="PA8" s="64"/>
-      <c r="PB8" s="64" t="s">
+      <c r="OZ8" s="62"/>
+      <c r="PA8" s="62"/>
+      <c r="PB8" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="PC8" s="64"/>
-      <c r="PD8" s="64"/>
-      <c r="PE8" s="64" t="s">
+      <c r="PC8" s="62"/>
+      <c r="PD8" s="62"/>
+      <c r="PE8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="PF8" s="64"/>
-      <c r="PG8" s="64"/>
-      <c r="PH8" s="64" t="s">
+      <c r="PF8" s="62"/>
+      <c r="PG8" s="62"/>
+      <c r="PH8" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="PI8" s="64"/>
-      <c r="PJ8" s="64"/>
-      <c r="PK8" s="64" t="s">
+      <c r="PI8" s="62"/>
+      <c r="PJ8" s="62"/>
+      <c r="PK8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="PL8" s="64"/>
-      <c r="PM8" s="64"/>
-      <c r="PN8" s="64" t="s">
+      <c r="PL8" s="62"/>
+      <c r="PM8" s="62"/>
+      <c r="PN8" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="PO8" s="64"/>
-      <c r="PP8" s="64"/>
-      <c r="PQ8" s="64" t="s">
+      <c r="PO8" s="62"/>
+      <c r="PP8" s="62"/>
+      <c r="PQ8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="PR8" s="64"/>
-      <c r="PS8" s="64"/>
-      <c r="PT8" s="64" t="s">
+      <c r="PR8" s="62"/>
+      <c r="PS8" s="62"/>
+      <c r="PT8" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="PU8" s="64"/>
-      <c r="PV8" s="64"/>
-      <c r="PW8" s="64" t="s">
+      <c r="PU8" s="62"/>
+      <c r="PV8" s="62"/>
+      <c r="PW8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="PX8" s="64"/>
-      <c r="PY8" s="64"/>
-      <c r="PZ8" s="64" t="s">
+      <c r="PX8" s="62"/>
+      <c r="PY8" s="62"/>
+      <c r="PZ8" s="62" t="s">
         <v>187</v>
       </c>
-      <c r="QA8" s="64"/>
-      <c r="QB8" s="64"/>
-      <c r="QC8" s="64" t="s">
+      <c r="QA8" s="62"/>
+      <c r="QB8" s="62"/>
+      <c r="QC8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="QD8" s="64"/>
-      <c r="QE8" s="64"/>
-      <c r="QF8" s="64" t="s">
+      <c r="QD8" s="62"/>
+      <c r="QE8" s="62"/>
+      <c r="QF8" s="62" t="s">
         <v>188</v>
       </c>
-      <c r="QG8" s="64"/>
-      <c r="QH8" s="64"/>
-      <c r="QI8" s="64" t="s">
+      <c r="QG8" s="62"/>
+      <c r="QH8" s="62"/>
+      <c r="QI8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="QJ8" s="64"/>
-      <c r="QK8" s="64"/>
-      <c r="QL8" s="64" t="s">
+      <c r="QJ8" s="62"/>
+      <c r="QK8" s="62"/>
+      <c r="QL8" s="62" t="s">
         <v>189</v>
       </c>
-      <c r="QM8" s="64"/>
-      <c r="QN8" s="64"/>
-      <c r="QO8" s="64" t="s">
+      <c r="QM8" s="62"/>
+      <c r="QN8" s="62"/>
+      <c r="QO8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="QP8" s="64"/>
-      <c r="QQ8" s="64"/>
-      <c r="QR8" s="64" t="s">
+      <c r="QP8" s="62"/>
+      <c r="QQ8" s="62"/>
+      <c r="QR8" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="QS8" s="64"/>
-      <c r="QT8" s="64"/>
-      <c r="QU8" s="64" t="s">
+      <c r="QS8" s="62"/>
+      <c r="QT8" s="62"/>
+      <c r="QU8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="QV8" s="64"/>
-      <c r="QW8" s="64"/>
-      <c r="QX8" s="64" t="s">
+      <c r="QV8" s="62"/>
+      <c r="QW8" s="62"/>
+      <c r="QX8" s="62" t="s">
         <v>191</v>
       </c>
-      <c r="QY8" s="64"/>
-      <c r="QZ8" s="64"/>
-      <c r="RA8" s="64" t="s">
+      <c r="QY8" s="62"/>
+      <c r="QZ8" s="62"/>
+      <c r="RA8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="RB8" s="64"/>
-      <c r="RC8" s="64"/>
-      <c r="RD8" s="64" t="s">
+      <c r="RB8" s="62"/>
+      <c r="RC8" s="62"/>
+      <c r="RD8" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="RE8" s="64"/>
-      <c r="RF8" s="64"/>
-      <c r="RG8" s="64" t="s">
+      <c r="RE8" s="62"/>
+      <c r="RF8" s="62"/>
+      <c r="RG8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="RH8" s="64"/>
-      <c r="RI8" s="64"/>
-      <c r="RJ8" s="64" t="s">
+      <c r="RH8" s="62"/>
+      <c r="RI8" s="62"/>
+      <c r="RJ8" s="62" t="s">
         <v>193</v>
       </c>
-      <c r="RK8" s="64"/>
-      <c r="RL8" s="64"/>
-      <c r="RM8" s="64" t="s">
+      <c r="RK8" s="62"/>
+      <c r="RL8" s="62"/>
+      <c r="RM8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="RN8" s="64"/>
-      <c r="RO8" s="64"/>
-      <c r="RP8" s="64" t="s">
+      <c r="RN8" s="62"/>
+      <c r="RO8" s="62"/>
+      <c r="RP8" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="RQ8" s="64"/>
-      <c r="RR8" s="64"/>
-      <c r="RS8" s="64" t="s">
+      <c r="RQ8" s="62"/>
+      <c r="RR8" s="62"/>
+      <c r="RS8" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="RT8" s="64"/>
-      <c r="RU8" s="64"/>
+      <c r="RT8" s="62"/>
+      <c r="RU8" s="62"/>
     </row>
     <row r="9" spans="1:489" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A9" s="71"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="67"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="64"/>
       <c r="J9" s="4" t="s">
         <v>96</v>
       </c>
@@ -6798,39 +7012,39 @@
       </c>
     </row>
     <row r="34" spans="1:78" ht="15" customHeight="1">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="69" t="s">
         <v>243</v>
       </c>
-      <c r="B34" s="65"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
     </row>
     <row r="35" spans="1:78">
-      <c r="A35" s="65"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
     </row>
     <row r="36" spans="1:78" ht="78.75" customHeight="1">
-      <c r="A36" s="65"/>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
+      <c r="A36" s="69"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
     </row>
     <row r="38" spans="1:78">
       <c r="A38" s="1" t="s">
@@ -7158,120 +7372,120 @@
     <row r="47" spans="1:78">
       <c r="A47" s="43"/>
       <c r="B47" s="45"/>
-      <c r="C47" s="62">
+      <c r="C47" s="70">
         <v>1998</v>
       </c>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="62">
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="70">
         <v>1999</v>
       </c>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
-      <c r="K47" s="62">
+      <c r="H47" s="71"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="71"/>
+      <c r="K47" s="70">
         <v>2000</v>
       </c>
-      <c r="L47" s="63"/>
-      <c r="M47" s="63"/>
-      <c r="N47" s="63"/>
-      <c r="O47" s="62">
+      <c r="L47" s="71"/>
+      <c r="M47" s="71"/>
+      <c r="N47" s="71"/>
+      <c r="O47" s="70">
         <v>2001</v>
       </c>
-      <c r="P47" s="63"/>
-      <c r="Q47" s="63"/>
-      <c r="R47" s="63"/>
-      <c r="S47" s="62">
+      <c r="P47" s="71"/>
+      <c r="Q47" s="71"/>
+      <c r="R47" s="71"/>
+      <c r="S47" s="70">
         <v>2002</v>
       </c>
-      <c r="T47" s="63"/>
-      <c r="U47" s="63"/>
-      <c r="V47" s="63"/>
-      <c r="W47" s="62">
+      <c r="T47" s="71"/>
+      <c r="U47" s="71"/>
+      <c r="V47" s="71"/>
+      <c r="W47" s="70">
         <v>2003</v>
       </c>
-      <c r="X47" s="63"/>
-      <c r="Y47" s="63"/>
-      <c r="Z47" s="63"/>
-      <c r="AA47" s="62">
+      <c r="X47" s="71"/>
+      <c r="Y47" s="71"/>
+      <c r="Z47" s="71"/>
+      <c r="AA47" s="70">
         <v>2004</v>
       </c>
-      <c r="AB47" s="63"/>
-      <c r="AC47" s="63"/>
-      <c r="AD47" s="63"/>
-      <c r="AE47" s="62">
+      <c r="AB47" s="71"/>
+      <c r="AC47" s="71"/>
+      <c r="AD47" s="71"/>
+      <c r="AE47" s="70">
         <v>2005</v>
       </c>
-      <c r="AF47" s="63"/>
-      <c r="AG47" s="63"/>
-      <c r="AH47" s="63"/>
-      <c r="AI47" s="62">
+      <c r="AF47" s="71"/>
+      <c r="AG47" s="71"/>
+      <c r="AH47" s="71"/>
+      <c r="AI47" s="70">
         <v>2006</v>
       </c>
-      <c r="AJ47" s="63"/>
-      <c r="AK47" s="63"/>
-      <c r="AL47" s="63"/>
-      <c r="AM47" s="62">
+      <c r="AJ47" s="71"/>
+      <c r="AK47" s="71"/>
+      <c r="AL47" s="71"/>
+      <c r="AM47" s="70">
         <v>2007</v>
       </c>
-      <c r="AN47" s="63"/>
-      <c r="AO47" s="63"/>
-      <c r="AP47" s="63"/>
-      <c r="AQ47" s="62">
+      <c r="AN47" s="71"/>
+      <c r="AO47" s="71"/>
+      <c r="AP47" s="71"/>
+      <c r="AQ47" s="70">
         <v>2008</v>
       </c>
-      <c r="AR47" s="63"/>
-      <c r="AS47" s="63"/>
-      <c r="AT47" s="63"/>
-      <c r="AU47" s="62">
+      <c r="AR47" s="71"/>
+      <c r="AS47" s="71"/>
+      <c r="AT47" s="71"/>
+      <c r="AU47" s="70">
         <v>2009</v>
       </c>
-      <c r="AV47" s="63"/>
-      <c r="AW47" s="63"/>
-      <c r="AX47" s="63"/>
-      <c r="AY47" s="62">
+      <c r="AV47" s="71"/>
+      <c r="AW47" s="71"/>
+      <c r="AX47" s="71"/>
+      <c r="AY47" s="70">
         <v>2010</v>
       </c>
-      <c r="AZ47" s="63"/>
-      <c r="BA47" s="63"/>
-      <c r="BB47" s="63"/>
-      <c r="BC47" s="62">
+      <c r="AZ47" s="71"/>
+      <c r="BA47" s="71"/>
+      <c r="BB47" s="71"/>
+      <c r="BC47" s="70">
         <v>2011</v>
       </c>
-      <c r="BD47" s="63"/>
-      <c r="BE47" s="63"/>
-      <c r="BF47" s="63"/>
-      <c r="BG47" s="62">
+      <c r="BD47" s="71"/>
+      <c r="BE47" s="71"/>
+      <c r="BF47" s="71"/>
+      <c r="BG47" s="70">
         <v>2012</v>
       </c>
-      <c r="BH47" s="63"/>
-      <c r="BI47" s="63"/>
-      <c r="BJ47" s="63"/>
-      <c r="BK47" s="62">
+      <c r="BH47" s="71"/>
+      <c r="BI47" s="71"/>
+      <c r="BJ47" s="71"/>
+      <c r="BK47" s="70">
         <v>2013</v>
       </c>
-      <c r="BL47" s="63"/>
-      <c r="BM47" s="63"/>
-      <c r="BN47" s="63"/>
-      <c r="BO47" s="62">
+      <c r="BL47" s="71"/>
+      <c r="BM47" s="71"/>
+      <c r="BN47" s="71"/>
+      <c r="BO47" s="70">
         <v>2014</v>
       </c>
-      <c r="BP47" s="63"/>
-      <c r="BQ47" s="63"/>
-      <c r="BR47" s="63"/>
-      <c r="BS47" s="62">
+      <c r="BP47" s="71"/>
+      <c r="BQ47" s="71"/>
+      <c r="BR47" s="71"/>
+      <c r="BS47" s="70">
         <v>2015</v>
       </c>
-      <c r="BT47" s="63"/>
-      <c r="BU47" s="63"/>
-      <c r="BV47" s="63"/>
-      <c r="BW47" s="62">
+      <c r="BT47" s="71"/>
+      <c r="BU47" s="71"/>
+      <c r="BV47" s="71"/>
+      <c r="BW47" s="70">
         <v>2016</v>
       </c>
-      <c r="BX47" s="63"/>
-      <c r="BY47" s="63"/>
-      <c r="BZ47" s="63"/>
+      <c r="BX47" s="71"/>
+      <c r="BY47" s="71"/>
+      <c r="BZ47" s="71"/>
     </row>
     <row r="48" spans="1:78">
       <c r="A48" s="44" t="s">
@@ -12321,8 +12535,1172 @@
         <v>2.1</v>
       </c>
     </row>
+    <row r="80" spans="1:78">
+      <c r="A80" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A82" s="72" t="s">
+        <v>461</v>
+      </c>
+      <c r="B82" s="72" t="s">
+        <v>462</v>
+      </c>
+      <c r="C82" s="72" t="s">
+        <v>463</v>
+      </c>
+      <c r="D82" s="72" t="s">
+        <v>464</v>
+      </c>
+      <c r="E82" s="72" t="s">
+        <v>465</v>
+      </c>
+      <c r="F82" s="72" t="s">
+        <v>466</v>
+      </c>
+      <c r="G82" s="72" t="s">
+        <v>467</v>
+      </c>
+      <c r="H82" s="72" t="s">
+        <v>468</v>
+      </c>
+      <c r="I82" s="72" t="s">
+        <v>469</v>
+      </c>
+      <c r="J82" s="72" t="s">
+        <v>470</v>
+      </c>
+      <c r="K82" s="72" t="s">
+        <v>471</v>
+      </c>
+      <c r="L82" s="72" t="s">
+        <v>472</v>
+      </c>
+      <c r="M82" s="72" t="s">
+        <v>473</v>
+      </c>
+      <c r="N82" s="72" t="s">
+        <v>474</v>
+      </c>
+      <c r="O82" s="72" t="s">
+        <v>475</v>
+      </c>
+      <c r="P82" s="72" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q82" s="72" t="s">
+        <v>477</v>
+      </c>
+      <c r="R82" s="72" t="s">
+        <v>478</v>
+      </c>
+      <c r="S82" s="72" t="s">
+        <v>479</v>
+      </c>
+      <c r="T82" s="72" t="s">
+        <v>480</v>
+      </c>
+      <c r="U82" s="72" t="s">
+        <v>481</v>
+      </c>
+      <c r="V82" s="72" t="s">
+        <v>482</v>
+      </c>
+      <c r="W82" s="72" t="s">
+        <v>483</v>
+      </c>
+      <c r="X82" s="25"/>
+    </row>
+    <row r="83" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A83" s="73">
+        <v>3</v>
+      </c>
+      <c r="B83" s="73">
+        <v>35</v>
+      </c>
+      <c r="C83" s="73">
+        <v>25</v>
+      </c>
+      <c r="D83" s="73">
+        <v>29.368358910000001</v>
+      </c>
+      <c r="E83" s="73">
+        <v>0</v>
+      </c>
+      <c r="F83" s="73">
+        <v>1</v>
+      </c>
+      <c r="G83" s="73">
+        <v>1</v>
+      </c>
+      <c r="H83" s="73">
+        <v>1</v>
+      </c>
+      <c r="I83" s="73">
+        <v>20</v>
+      </c>
+      <c r="J83" s="73">
+        <v>0</v>
+      </c>
+      <c r="K83" s="73">
+        <v>2.0698400000000001E-4</v>
+      </c>
+      <c r="L83" s="73">
+        <v>6.5446134000000003E-2</v>
+      </c>
+      <c r="M83" s="74">
+        <v>5.0300000000000001E-6</v>
+      </c>
+      <c r="N83" s="74">
+        <v>6.8999999999999997E-5</v>
+      </c>
+      <c r="O83" s="73">
+        <v>3.5213380000000002E-3</v>
+      </c>
+      <c r="P83" s="73">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="73">
+        <v>0</v>
+      </c>
+      <c r="R83" s="73">
+        <v>0</v>
+      </c>
+      <c r="S83" s="73">
+        <v>0</v>
+      </c>
+      <c r="T83" s="73">
+        <v>0</v>
+      </c>
+      <c r="U83" s="73">
+        <v>0.93070390800000002</v>
+      </c>
+      <c r="V83" s="73">
+        <v>0</v>
+      </c>
+      <c r="W83" s="74">
+        <v>4.7599999999999998E-5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A84" s="75">
+        <v>3</v>
+      </c>
+      <c r="B84" s="75">
+        <v>36</v>
+      </c>
+      <c r="C84" s="75">
+        <v>25</v>
+      </c>
+      <c r="D84" s="75">
+        <v>29.48642267</v>
+      </c>
+      <c r="E84" s="75">
+        <v>0</v>
+      </c>
+      <c r="F84" s="75">
+        <v>1</v>
+      </c>
+      <c r="G84" s="75">
+        <v>1</v>
+      </c>
+      <c r="H84" s="75">
+        <v>1</v>
+      </c>
+      <c r="I84" s="75">
+        <v>20</v>
+      </c>
+      <c r="J84" s="75">
+        <v>0</v>
+      </c>
+      <c r="K84" s="75">
+        <v>1.8755900000000001E-4</v>
+      </c>
+      <c r="L84" s="75">
+        <v>0.13525103799999999</v>
+      </c>
+      <c r="M84" s="76">
+        <v>7.7800000000000001E-7</v>
+      </c>
+      <c r="N84" s="76">
+        <v>6.2500000000000001E-5</v>
+      </c>
+      <c r="O84" s="75">
+        <v>2.9583801E-2</v>
+      </c>
+      <c r="P84" s="75">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="75">
+        <v>0</v>
+      </c>
+      <c r="R84" s="75">
+        <v>0</v>
+      </c>
+      <c r="S84" s="75">
+        <v>0</v>
+      </c>
+      <c r="T84" s="75">
+        <v>0</v>
+      </c>
+      <c r="U84" s="75">
+        <v>0.83486074899999996</v>
+      </c>
+      <c r="V84" s="75">
+        <v>0</v>
+      </c>
+      <c r="W84" s="76">
+        <v>5.3600000000000002E-5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A85" s="73">
+        <v>3</v>
+      </c>
+      <c r="B85" s="73">
+        <v>37</v>
+      </c>
+      <c r="C85" s="73">
+        <v>25</v>
+      </c>
+      <c r="D85" s="73">
+        <v>29.604486420000001</v>
+      </c>
+      <c r="E85" s="73">
+        <v>0</v>
+      </c>
+      <c r="F85" s="73">
+        <v>1</v>
+      </c>
+      <c r="G85" s="73">
+        <v>1</v>
+      </c>
+      <c r="H85" s="73">
+        <v>1</v>
+      </c>
+      <c r="I85" s="73">
+        <v>20</v>
+      </c>
+      <c r="J85" s="73">
+        <v>0</v>
+      </c>
+      <c r="K85" s="73">
+        <v>1.66379E-4</v>
+      </c>
+      <c r="L85" s="73">
+        <v>0.16778886700000001</v>
+      </c>
+      <c r="M85" s="73">
+        <v>0</v>
+      </c>
+      <c r="N85" s="74">
+        <v>5.5399999999999998E-5</v>
+      </c>
+      <c r="O85" s="73">
+        <v>4.1817958000000002E-2</v>
+      </c>
+      <c r="P85" s="73">
+        <v>0</v>
+      </c>
+      <c r="Q85" s="73">
+        <v>0</v>
+      </c>
+      <c r="R85" s="73">
+        <v>0</v>
+      </c>
+      <c r="S85" s="73">
+        <v>0</v>
+      </c>
+      <c r="T85" s="73">
+        <v>0</v>
+      </c>
+      <c r="U85" s="73">
+        <v>0.79008697100000003</v>
+      </c>
+      <c r="V85" s="73">
+        <v>0</v>
+      </c>
+      <c r="W85" s="74">
+        <v>8.4400000000000005E-5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A86" s="75">
+        <v>3</v>
+      </c>
+      <c r="B86" s="75">
+        <v>38</v>
+      </c>
+      <c r="C86" s="75">
+        <v>25</v>
+      </c>
+      <c r="D86" s="75">
+        <v>29.722550179999999</v>
+      </c>
+      <c r="E86" s="75">
+        <v>0</v>
+      </c>
+      <c r="F86" s="75">
+        <v>1</v>
+      </c>
+      <c r="G86" s="75">
+        <v>1</v>
+      </c>
+      <c r="H86" s="75">
+        <v>1</v>
+      </c>
+      <c r="I86" s="75">
+        <v>20</v>
+      </c>
+      <c r="J86" s="75">
+        <v>8.26708E-4</v>
+      </c>
+      <c r="K86" s="75">
+        <v>1.4451199999999999E-4</v>
+      </c>
+      <c r="L86" s="75">
+        <v>0.16697783299999999</v>
+      </c>
+      <c r="M86" s="75">
+        <v>0</v>
+      </c>
+      <c r="N86" s="76">
+        <v>4.8099999999999997E-5</v>
+      </c>
+      <c r="O86" s="75">
+        <v>4.1753132999999998E-2</v>
+      </c>
+      <c r="P86" s="75">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="75">
+        <v>0</v>
+      </c>
+      <c r="R86" s="75">
+        <v>0</v>
+      </c>
+      <c r="S86" s="75">
+        <v>0</v>
+      </c>
+      <c r="T86" s="75">
+        <v>0</v>
+      </c>
+      <c r="U86" s="75">
+        <v>0.79011126899999995</v>
+      </c>
+      <c r="V86" s="75">
+        <v>0</v>
+      </c>
+      <c r="W86" s="75">
+        <v>1.383E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A89" s="72" t="s">
+        <v>461</v>
+      </c>
+      <c r="B89" s="72" t="s">
+        <v>484</v>
+      </c>
+      <c r="C89" s="72" t="s">
+        <v>485</v>
+      </c>
+      <c r="D89" s="72">
+        <v>4477696</v>
+      </c>
+      <c r="E89" s="72">
+        <v>4442130</v>
+      </c>
+      <c r="F89" s="72">
+        <v>4453535</v>
+      </c>
+      <c r="G89" s="72">
+        <v>4409545</v>
+      </c>
+      <c r="H89" s="72">
+        <v>4479989</v>
+      </c>
+      <c r="I89" s="72">
+        <v>4483174</v>
+      </c>
+      <c r="J89" s="72">
+        <v>4310398</v>
+      </c>
+      <c r="K89" s="72">
+        <v>4475758</v>
+      </c>
+      <c r="L89" s="72">
+        <v>4483015</v>
+      </c>
+      <c r="M89" s="72">
+        <v>1023075</v>
+      </c>
+      <c r="N89" s="72">
+        <v>4467992</v>
+      </c>
+      <c r="O89" s="72">
+        <v>4447416</v>
+      </c>
+      <c r="P89" s="72">
+        <v>4396235</v>
+      </c>
+      <c r="Q89" s="72">
+        <v>4452538</v>
+      </c>
+      <c r="R89" s="72">
+        <v>4479603</v>
+      </c>
+      <c r="S89" s="72">
+        <v>4443574</v>
+      </c>
+      <c r="T89" s="72">
+        <v>1008348</v>
+      </c>
+      <c r="U89" s="72">
+        <v>4465803</v>
+      </c>
+      <c r="V89" s="72">
+        <v>1696853</v>
+      </c>
+      <c r="W89" s="25"/>
+    </row>
+    <row r="90" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A90" s="73">
+        <v>2</v>
+      </c>
+      <c r="B90" s="73">
+        <v>59</v>
+      </c>
+      <c r="C90" s="73">
+        <v>262</v>
+      </c>
+      <c r="D90" s="73">
+        <v>5.9274990000000001E-3</v>
+      </c>
+      <c r="E90" s="73">
+        <v>2.6355340000000001E-3</v>
+      </c>
+      <c r="F90" s="73">
+        <v>6.9169990000000001E-3</v>
+      </c>
+      <c r="G90" s="73">
+        <v>1.3904499999999999E-4</v>
+      </c>
+      <c r="H90" s="73">
+        <v>0.45107575999999999</v>
+      </c>
+      <c r="I90" s="73">
+        <v>0</v>
+      </c>
+      <c r="J90" s="73">
+        <v>1.17753E-4</v>
+      </c>
+      <c r="K90" s="73">
+        <v>0.20354787899999999</v>
+      </c>
+      <c r="L90" s="73">
+        <v>2.0555999999999999E-3</v>
+      </c>
+      <c r="M90" s="73">
+        <v>3.0082809999999998E-3</v>
+      </c>
+      <c r="N90" s="73">
+        <v>8.0592921999999997E-2</v>
+      </c>
+      <c r="O90" s="74">
+        <v>2.3799999999999999E-5</v>
+      </c>
+      <c r="P90" s="73">
+        <v>9.5061400000000002E-4</v>
+      </c>
+      <c r="Q90" s="73">
+        <v>1.3842209999999999E-3</v>
+      </c>
+      <c r="R90" s="73">
+        <v>1.0308729000000001E-2</v>
+      </c>
+      <c r="S90" s="73">
+        <v>0</v>
+      </c>
+      <c r="T90" s="73">
+        <v>1.1927299999999999E-3</v>
+      </c>
+      <c r="U90" s="73">
+        <v>0</v>
+      </c>
+      <c r="V90" s="73">
+        <v>2.5571999999999999E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A91" s="75">
+        <v>2</v>
+      </c>
+      <c r="B91" s="75">
+        <v>73</v>
+      </c>
+      <c r="C91" s="75">
+        <v>262</v>
+      </c>
+      <c r="D91" s="75">
+        <v>1.6550118999999999E-2</v>
+      </c>
+      <c r="E91" s="75">
+        <v>6.086836E-3</v>
+      </c>
+      <c r="F91" s="75">
+        <v>9.0947560000000007E-3</v>
+      </c>
+      <c r="G91" s="75">
+        <v>2.49008E-4</v>
+      </c>
+      <c r="H91" s="75">
+        <v>0.50548730600000003</v>
+      </c>
+      <c r="I91" s="75">
+        <v>1.5042219999999999E-3</v>
+      </c>
+      <c r="J91" s="75">
+        <v>2.31208E-4</v>
+      </c>
+      <c r="K91" s="75">
+        <v>9.0964627000000006E-2</v>
+      </c>
+      <c r="L91" s="75">
+        <v>2.262525E-3</v>
+      </c>
+      <c r="M91" s="75">
+        <v>2.5396730000000001E-3</v>
+      </c>
+      <c r="N91" s="75">
+        <v>5.6683187000000003E-2</v>
+      </c>
+      <c r="O91" s="75">
+        <v>1.7504838000000002E-2</v>
+      </c>
+      <c r="P91" s="75">
+        <v>1.650966E-3</v>
+      </c>
+      <c r="Q91" s="75">
+        <v>1.8998610000000001E-3</v>
+      </c>
+      <c r="R91" s="75">
+        <v>1.0040403E-2</v>
+      </c>
+      <c r="S91" s="75">
+        <v>6.8909519999999997E-3</v>
+      </c>
+      <c r="T91" s="75">
+        <v>1.0329390000000001E-3</v>
+      </c>
+      <c r="U91" s="75">
+        <v>0</v>
+      </c>
+      <c r="V91" s="75">
+        <v>3.7968110000000002E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A92" s="73">
+        <v>2</v>
+      </c>
+      <c r="B92" s="73">
+        <v>87</v>
+      </c>
+      <c r="C92" s="73">
+        <v>262</v>
+      </c>
+      <c r="D92" s="73">
+        <v>1.7835073999999999E-2</v>
+      </c>
+      <c r="E92" s="73">
+        <v>7.6499339999999997E-3</v>
+      </c>
+      <c r="F92" s="73">
+        <v>8.1510369999999999E-3</v>
+      </c>
+      <c r="G92" s="73">
+        <v>2.8239500000000001E-4</v>
+      </c>
+      <c r="H92" s="73">
+        <v>0.72203508599999999</v>
+      </c>
+      <c r="I92" s="73">
+        <v>7.7239199999999996E-3</v>
+      </c>
+      <c r="J92" s="73">
+        <v>2.9477399999999998E-4</v>
+      </c>
+      <c r="K92" s="73">
+        <v>6.1359282000000001E-2</v>
+      </c>
+      <c r="L92" s="73">
+        <v>1.4889910000000001E-3</v>
+      </c>
+      <c r="M92" s="73">
+        <v>1.0320419999999999E-3</v>
+      </c>
+      <c r="N92" s="73">
+        <v>3.2703910000000003E-2</v>
+      </c>
+      <c r="O92" s="73">
+        <v>0</v>
+      </c>
+      <c r="P92" s="73">
+        <v>1.6983549999999999E-3</v>
+      </c>
+      <c r="Q92" s="73">
+        <v>1.883909E-3</v>
+      </c>
+      <c r="R92" s="73">
+        <v>6.6217469999999999E-3</v>
+      </c>
+      <c r="S92" s="73">
+        <v>2.1107900999999998E-2</v>
+      </c>
+      <c r="T92" s="73">
+        <v>4.2338E-4</v>
+      </c>
+      <c r="U92" s="74">
+        <v>7.9000000000000006E-6</v>
+      </c>
+      <c r="V92" s="73">
+        <v>3.8441080000000002E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A93" s="75">
+        <v>2</v>
+      </c>
+      <c r="B93" s="75">
+        <v>101</v>
+      </c>
+      <c r="C93" s="75">
+        <v>262</v>
+      </c>
+      <c r="D93" s="75">
+        <v>4.8287199999999999E-3</v>
+      </c>
+      <c r="E93" s="75">
+        <v>8.0598760000000005E-3</v>
+      </c>
+      <c r="F93" s="75">
+        <v>7.3449689999999998E-3</v>
+      </c>
+      <c r="G93" s="75">
+        <v>2.90406E-4</v>
+      </c>
+      <c r="H93" s="75">
+        <v>0.25782157900000002</v>
+      </c>
+      <c r="I93" s="75">
+        <v>3.8139850000000002E-3</v>
+      </c>
+      <c r="J93" s="75">
+        <v>3.41238E-4</v>
+      </c>
+      <c r="K93" s="75">
+        <v>1.80676E-2</v>
+      </c>
+      <c r="L93" s="75">
+        <v>8.3995300000000005E-4</v>
+      </c>
+      <c r="M93" s="75">
+        <v>1.5578099999999999E-4</v>
+      </c>
+      <c r="N93" s="75">
+        <v>2.293125E-3</v>
+      </c>
+      <c r="O93" s="75">
+        <v>6.8269299999999995E-4</v>
+      </c>
+      <c r="P93" s="75">
+        <v>1.499626E-3</v>
+      </c>
+      <c r="Q93" s="75">
+        <v>1.7775149999999999E-3</v>
+      </c>
+      <c r="R93" s="75">
+        <v>3.7660279999999998E-3</v>
+      </c>
+      <c r="S93" s="75">
+        <v>1.610591E-3</v>
+      </c>
+      <c r="T93" s="76">
+        <v>1.2799999999999999E-5</v>
+      </c>
+      <c r="U93" s="76">
+        <v>1.34E-5</v>
+      </c>
+      <c r="V93" s="75">
+        <v>3.5811390000000001E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26">
+      <c r="A94" s="25"/>
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="25"/>
+      <c r="H94" s="25"/>
+      <c r="I94" s="25"/>
+      <c r="J94" s="25"/>
+      <c r="K94" s="25"/>
+      <c r="L94" s="25"/>
+      <c r="M94" s="25"/>
+      <c r="N94" s="25"/>
+      <c r="O94" s="25"/>
+      <c r="P94" s="25"/>
+      <c r="Q94" s="25"/>
+      <c r="R94" s="25"/>
+    </row>
+    <row r="96" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A96" s="72" t="s">
+        <v>461</v>
+      </c>
+      <c r="B96" s="72" t="s">
+        <v>486</v>
+      </c>
+      <c r="C96" s="72" t="s">
+        <v>487</v>
+      </c>
+      <c r="D96" s="72" t="s">
+        <v>488</v>
+      </c>
+      <c r="E96" s="72" t="s">
+        <v>489</v>
+      </c>
+      <c r="F96" s="72" t="s">
+        <v>490</v>
+      </c>
+      <c r="G96" s="72" t="s">
+        <v>491</v>
+      </c>
+      <c r="H96" s="72" t="s">
+        <v>492</v>
+      </c>
+      <c r="I96" s="72" t="s">
+        <v>493</v>
+      </c>
+      <c r="J96" s="72" t="s">
+        <v>494</v>
+      </c>
+      <c r="K96" s="72" t="s">
+        <v>495</v>
+      </c>
+      <c r="L96" s="72" t="s">
+        <v>496</v>
+      </c>
+      <c r="M96" s="72" t="s">
+        <v>497</v>
+      </c>
+      <c r="N96" s="72" t="s">
+        <v>498</v>
+      </c>
+      <c r="O96" s="72" t="s">
+        <v>499</v>
+      </c>
+      <c r="P96" s="72" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q96" s="72" t="s">
+        <v>501</v>
+      </c>
+      <c r="R96" s="72" t="s">
+        <v>502</v>
+      </c>
+      <c r="S96" s="72" t="s">
+        <v>503</v>
+      </c>
+      <c r="T96" s="72" t="s">
+        <v>504</v>
+      </c>
+      <c r="U96" s="72" t="s">
+        <v>505</v>
+      </c>
+      <c r="V96" s="72" t="s">
+        <v>506</v>
+      </c>
+      <c r="W96" s="72" t="s">
+        <v>507</v>
+      </c>
+      <c r="X96" s="72" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y96" s="72" t="s">
+        <v>509</v>
+      </c>
+      <c r="Z96" s="25"/>
+    </row>
+    <row r="97" spans="1:25" ht="15.75" thickBot="1">
+      <c r="A97" s="73">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B97" s="73">
+        <v>0</v>
+      </c>
+      <c r="C97" s="74">
+        <v>4.0599999999999998E-5</v>
+      </c>
+      <c r="D97" s="73">
+        <v>1.946433E-3</v>
+      </c>
+      <c r="E97" s="73">
+        <v>0</v>
+      </c>
+      <c r="F97" s="73">
+        <v>1.0729822999999999E-2</v>
+      </c>
+      <c r="G97" s="73">
+        <v>4.1896541000000002E-2</v>
+      </c>
+      <c r="H97" s="73">
+        <v>7.7626300000000002E-4</v>
+      </c>
+      <c r="I97" s="73">
+        <v>0</v>
+      </c>
+      <c r="J97" s="73">
+        <v>5.1525599999999996E-4</v>
+      </c>
+      <c r="K97" s="73">
+        <v>0.49333814399999998</v>
+      </c>
+      <c r="L97" s="73">
+        <v>1.938111E-3</v>
+      </c>
+      <c r="M97" s="73">
+        <v>1.2953507E-2</v>
+      </c>
+      <c r="N97" s="73">
+        <v>5.0174400000000004E-4</v>
+      </c>
+      <c r="O97" s="73">
+        <v>9.0231939999999997E-2</v>
+      </c>
+      <c r="P97" s="74">
+        <v>9.2800000000000006E-5</v>
+      </c>
+      <c r="Q97" s="73">
+        <v>2.9041174999999999E-2</v>
+      </c>
+      <c r="R97" s="73">
+        <v>6.7826639999999999E-3</v>
+      </c>
+      <c r="S97" s="74">
+        <v>7.3499999999999998E-5</v>
+      </c>
+      <c r="T97" s="73">
+        <v>0</v>
+      </c>
+      <c r="U97" s="73">
+        <v>2.242033E-3</v>
+      </c>
+      <c r="V97" s="73">
+        <v>1.7755119999999999E-3</v>
+      </c>
+      <c r="W97" s="73">
+        <v>4.9386229999999996E-3</v>
+      </c>
+      <c r="X97" s="73">
+        <v>5.8052799999999997E-4</v>
+      </c>
+      <c r="Y97" s="73">
+        <v>3.4587442000000003E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25" ht="15.75" thickBot="1">
+      <c r="A98" s="75">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B98" s="75">
+        <v>14</v>
+      </c>
+      <c r="C98" s="75">
+        <v>1.562461E-3</v>
+      </c>
+      <c r="D98" s="75">
+        <v>1.2770030000000001E-3</v>
+      </c>
+      <c r="E98" s="75">
+        <v>6.4541299999999995E-4</v>
+      </c>
+      <c r="F98" s="75">
+        <v>7.2902349999999999E-3</v>
+      </c>
+      <c r="G98" s="75">
+        <v>0</v>
+      </c>
+      <c r="H98" s="75">
+        <v>4.7252399999999999E-4</v>
+      </c>
+      <c r="I98" s="76">
+        <v>3.7100000000000001E-5</v>
+      </c>
+      <c r="J98" s="75">
+        <v>2.9523800000000002E-4</v>
+      </c>
+      <c r="K98" s="75">
+        <v>0.71350525499999995</v>
+      </c>
+      <c r="L98" s="75">
+        <v>6.5623920000000002E-3</v>
+      </c>
+      <c r="M98" s="75">
+        <v>1.1915082E-2</v>
+      </c>
+      <c r="N98" s="75">
+        <v>3.0565399999999998E-4</v>
+      </c>
+      <c r="O98" s="75">
+        <v>2.9839318E-2</v>
+      </c>
+      <c r="P98" s="76">
+        <v>7.75E-5</v>
+      </c>
+      <c r="Q98" s="75">
+        <v>2.0216921999999998E-2</v>
+      </c>
+      <c r="R98" s="75">
+        <v>4.4166819999999999E-3</v>
+      </c>
+      <c r="S98" s="76">
+        <v>8.0199999999999998E-5</v>
+      </c>
+      <c r="T98" s="76">
+        <v>2.5500000000000001E-6</v>
+      </c>
+      <c r="U98" s="75">
+        <v>1.7998529999999999E-3</v>
+      </c>
+      <c r="V98" s="75">
+        <v>1.516379E-3</v>
+      </c>
+      <c r="W98" s="75">
+        <v>2.8182569999999998E-3</v>
+      </c>
+      <c r="X98" s="75">
+        <v>3.5214000000000003E-4</v>
+      </c>
+      <c r="Y98" s="75">
+        <v>1.8032133999999998E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:25" ht="15.75" thickBot="1">
+      <c r="A99" s="73">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B99" s="73">
+        <v>28</v>
+      </c>
+      <c r="C99" s="73">
+        <v>3.5234820000000001E-3</v>
+      </c>
+      <c r="D99" s="73">
+        <v>1.5052799999999999E-3</v>
+      </c>
+      <c r="E99" s="73">
+        <v>1.8240649999999999E-3</v>
+      </c>
+      <c r="F99" s="73">
+        <v>8.8743980000000004E-3</v>
+      </c>
+      <c r="G99" s="73">
+        <v>2.1289333000000001E-2</v>
+      </c>
+      <c r="H99" s="73">
+        <v>5.1050900000000003E-4</v>
+      </c>
+      <c r="I99" s="73">
+        <v>1.02019E-4</v>
+      </c>
+      <c r="J99" s="73">
+        <v>2.95574E-4</v>
+      </c>
+      <c r="K99" s="73">
+        <v>0.65988184299999997</v>
+      </c>
+      <c r="L99" s="73">
+        <v>1.3712502999999999E-2</v>
+      </c>
+      <c r="M99" s="73">
+        <v>1.7759629999999998E-2</v>
+      </c>
+      <c r="N99" s="73">
+        <v>3.3933100000000001E-4</v>
+      </c>
+      <c r="O99" s="73">
+        <v>7.5271909999999999E-3</v>
+      </c>
+      <c r="P99" s="73">
+        <v>1.0993300000000001E-4</v>
+      </c>
+      <c r="Q99" s="73">
+        <v>2.4865589E-2</v>
+      </c>
+      <c r="R99" s="73">
+        <v>5.1579620000000003E-3</v>
+      </c>
+      <c r="S99" s="73">
+        <v>1.29004E-4</v>
+      </c>
+      <c r="T99" s="74">
+        <v>8.1799999999999996E-6</v>
+      </c>
+      <c r="U99" s="73">
+        <v>2.513506E-3</v>
+      </c>
+      <c r="V99" s="73">
+        <v>2.1619460000000001E-3</v>
+      </c>
+      <c r="W99" s="73">
+        <v>2.8500489999999999E-3</v>
+      </c>
+      <c r="X99" s="73">
+        <v>3.79823E-4</v>
+      </c>
+      <c r="Y99" s="73">
+        <v>1.7655562E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" ht="15.75" thickBot="1">
+      <c r="A100" s="75"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="25"/>
+      <c r="H100" s="25"/>
+      <c r="I100" s="25"/>
+      <c r="J100" s="25"/>
+      <c r="K100" s="25"/>
+      <c r="L100" s="25"/>
+      <c r="M100" s="25"/>
+      <c r="N100" s="25"/>
+      <c r="O100" s="25"/>
+      <c r="P100" s="25"/>
+      <c r="Q100" s="25"/>
+      <c r="R100" s="25"/>
+      <c r="S100" s="25"/>
+      <c r="T100" s="25"/>
+      <c r="U100" s="25"/>
+      <c r="V100" s="25"/>
+      <c r="W100" s="25"/>
+      <c r="X100" s="25"/>
+      <c r="Y100" s="25"/>
+    </row>
   </sheetData>
   <mergeCells count="130">
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="O47:R47"/>
+    <mergeCell ref="S47:V47"/>
+    <mergeCell ref="W47:Z47"/>
+    <mergeCell ref="AA47:AD47"/>
+    <mergeCell ref="AE47:AH47"/>
+    <mergeCell ref="AI47:AL47"/>
+    <mergeCell ref="AM47:AP47"/>
+    <mergeCell ref="BK47:BN47"/>
+    <mergeCell ref="BO47:BR47"/>
+    <mergeCell ref="BS47:BV47"/>
+    <mergeCell ref="BW47:BZ47"/>
+    <mergeCell ref="AQ47:AT47"/>
+    <mergeCell ref="AU47:AX47"/>
+    <mergeCell ref="AY47:BB47"/>
+    <mergeCell ref="BC47:BF47"/>
+    <mergeCell ref="BG47:BJ47"/>
+    <mergeCell ref="QX8:RC8"/>
+    <mergeCell ref="RD8:RI8"/>
+    <mergeCell ref="RJ8:RO8"/>
+    <mergeCell ref="RP8:RU8"/>
+    <mergeCell ref="A34:I36"/>
+    <mergeCell ref="PN8:PS8"/>
+    <mergeCell ref="PT8:PY8"/>
+    <mergeCell ref="PZ8:QE8"/>
+    <mergeCell ref="QF8:QK8"/>
+    <mergeCell ref="QL8:QQ8"/>
+    <mergeCell ref="QR8:QW8"/>
+    <mergeCell ref="OD8:OI8"/>
+    <mergeCell ref="OJ8:OO8"/>
+    <mergeCell ref="OP8:OU8"/>
+    <mergeCell ref="OV8:PA8"/>
+    <mergeCell ref="PB8:PG8"/>
+    <mergeCell ref="PH8:PM8"/>
+    <mergeCell ref="MT8:MY8"/>
+    <mergeCell ref="MZ8:NE8"/>
+    <mergeCell ref="NF8:NK8"/>
+    <mergeCell ref="NL8:NQ8"/>
+    <mergeCell ref="NR8:NW8"/>
+    <mergeCell ref="NX8:OC8"/>
+    <mergeCell ref="LJ8:LO8"/>
+    <mergeCell ref="LP8:LU8"/>
+    <mergeCell ref="LV8:MA8"/>
+    <mergeCell ref="MB8:MG8"/>
+    <mergeCell ref="MH8:MM8"/>
+    <mergeCell ref="MN8:MS8"/>
+    <mergeCell ref="JZ8:KE8"/>
+    <mergeCell ref="KF8:KK8"/>
+    <mergeCell ref="KL8:KQ8"/>
+    <mergeCell ref="KR8:KW8"/>
+    <mergeCell ref="KX8:LC8"/>
+    <mergeCell ref="LD8:LI8"/>
+    <mergeCell ref="IP8:IU8"/>
+    <mergeCell ref="IV8:JA8"/>
+    <mergeCell ref="JB8:JG8"/>
+    <mergeCell ref="JH8:JM8"/>
+    <mergeCell ref="JN8:JS8"/>
+    <mergeCell ref="JT8:JY8"/>
+    <mergeCell ref="HF8:HK8"/>
+    <mergeCell ref="HL8:HQ8"/>
+    <mergeCell ref="HR8:HW8"/>
+    <mergeCell ref="HX8:IC8"/>
+    <mergeCell ref="ID8:II8"/>
+    <mergeCell ref="IJ8:IO8"/>
+    <mergeCell ref="FV8:GA8"/>
+    <mergeCell ref="GB8:GG8"/>
+    <mergeCell ref="GH8:GM8"/>
+    <mergeCell ref="GN8:GS8"/>
+    <mergeCell ref="GT8:GY8"/>
+    <mergeCell ref="GZ8:HE8"/>
+    <mergeCell ref="EL8:EQ8"/>
+    <mergeCell ref="ER8:EW8"/>
+    <mergeCell ref="EX8:FC8"/>
+    <mergeCell ref="FD8:FI8"/>
+    <mergeCell ref="FJ8:FO8"/>
+    <mergeCell ref="FP8:FU8"/>
+    <mergeCell ref="DP8:DT8"/>
+    <mergeCell ref="DU8:DY8"/>
+    <mergeCell ref="DZ8:EE8"/>
+    <mergeCell ref="EF8:EK8"/>
+    <mergeCell ref="CB8:CF8"/>
+    <mergeCell ref="CG8:CK8"/>
+    <mergeCell ref="CL8:CP8"/>
+    <mergeCell ref="CQ8:CU8"/>
+    <mergeCell ref="CV8:CZ8"/>
+    <mergeCell ref="DA8:DE8"/>
+    <mergeCell ref="BW8:CA8"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="AD8:AH8"/>
+    <mergeCell ref="AI8:AM8"/>
+    <mergeCell ref="AN8:AR8"/>
+    <mergeCell ref="AS8:AW8"/>
+    <mergeCell ref="DF8:DJ8"/>
+    <mergeCell ref="DK8:DO8"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="AX8:BB8"/>
+    <mergeCell ref="BC8:BG8"/>
+    <mergeCell ref="BH8:BL8"/>
+    <mergeCell ref="BM8:BQ8"/>
+    <mergeCell ref="BR8:BV8"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:X3"/>
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="A3:A4"/>
@@ -12347,112 +13725,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="O8:S8"/>
     <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="AX8:BB8"/>
-    <mergeCell ref="BC8:BG8"/>
-    <mergeCell ref="BH8:BL8"/>
-    <mergeCell ref="BM8:BQ8"/>
-    <mergeCell ref="BR8:BV8"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:X3"/>
-    <mergeCell ref="BW8:CA8"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="AD8:AH8"/>
-    <mergeCell ref="AI8:AM8"/>
-    <mergeCell ref="AN8:AR8"/>
-    <mergeCell ref="AS8:AW8"/>
-    <mergeCell ref="DF8:DJ8"/>
-    <mergeCell ref="DK8:DO8"/>
-    <mergeCell ref="DP8:DT8"/>
-    <mergeCell ref="DU8:DY8"/>
-    <mergeCell ref="DZ8:EE8"/>
-    <mergeCell ref="EF8:EK8"/>
-    <mergeCell ref="CB8:CF8"/>
-    <mergeCell ref="CG8:CK8"/>
-    <mergeCell ref="CL8:CP8"/>
-    <mergeCell ref="CQ8:CU8"/>
-    <mergeCell ref="CV8:CZ8"/>
-    <mergeCell ref="DA8:DE8"/>
-    <mergeCell ref="FV8:GA8"/>
-    <mergeCell ref="GB8:GG8"/>
-    <mergeCell ref="GH8:GM8"/>
-    <mergeCell ref="GN8:GS8"/>
-    <mergeCell ref="GT8:GY8"/>
-    <mergeCell ref="GZ8:HE8"/>
-    <mergeCell ref="EL8:EQ8"/>
-    <mergeCell ref="ER8:EW8"/>
-    <mergeCell ref="EX8:FC8"/>
-    <mergeCell ref="FD8:FI8"/>
-    <mergeCell ref="FJ8:FO8"/>
-    <mergeCell ref="FP8:FU8"/>
-    <mergeCell ref="IP8:IU8"/>
-    <mergeCell ref="IV8:JA8"/>
-    <mergeCell ref="JB8:JG8"/>
-    <mergeCell ref="JH8:JM8"/>
-    <mergeCell ref="JN8:JS8"/>
-    <mergeCell ref="JT8:JY8"/>
-    <mergeCell ref="HF8:HK8"/>
-    <mergeCell ref="HL8:HQ8"/>
-    <mergeCell ref="HR8:HW8"/>
-    <mergeCell ref="HX8:IC8"/>
-    <mergeCell ref="ID8:II8"/>
-    <mergeCell ref="IJ8:IO8"/>
-    <mergeCell ref="LP8:LU8"/>
-    <mergeCell ref="LV8:MA8"/>
-    <mergeCell ref="MB8:MG8"/>
-    <mergeCell ref="MH8:MM8"/>
-    <mergeCell ref="MN8:MS8"/>
-    <mergeCell ref="JZ8:KE8"/>
-    <mergeCell ref="KF8:KK8"/>
-    <mergeCell ref="KL8:KQ8"/>
-    <mergeCell ref="KR8:KW8"/>
-    <mergeCell ref="KX8:LC8"/>
-    <mergeCell ref="LD8:LI8"/>
-    <mergeCell ref="QX8:RC8"/>
-    <mergeCell ref="RD8:RI8"/>
-    <mergeCell ref="RJ8:RO8"/>
-    <mergeCell ref="RP8:RU8"/>
-    <mergeCell ref="A34:I36"/>
-    <mergeCell ref="PN8:PS8"/>
-    <mergeCell ref="PT8:PY8"/>
-    <mergeCell ref="PZ8:QE8"/>
-    <mergeCell ref="QF8:QK8"/>
-    <mergeCell ref="QL8:QQ8"/>
-    <mergeCell ref="QR8:QW8"/>
-    <mergeCell ref="OD8:OI8"/>
-    <mergeCell ref="OJ8:OO8"/>
-    <mergeCell ref="OP8:OU8"/>
-    <mergeCell ref="OV8:PA8"/>
-    <mergeCell ref="PB8:PG8"/>
-    <mergeCell ref="PH8:PM8"/>
-    <mergeCell ref="MT8:MY8"/>
-    <mergeCell ref="MZ8:NE8"/>
-    <mergeCell ref="NF8:NK8"/>
-    <mergeCell ref="NL8:NQ8"/>
-    <mergeCell ref="NR8:NW8"/>
-    <mergeCell ref="NX8:OC8"/>
-    <mergeCell ref="LJ8:LO8"/>
-    <mergeCell ref="AM47:AP47"/>
-    <mergeCell ref="BK47:BN47"/>
-    <mergeCell ref="BO47:BR47"/>
-    <mergeCell ref="BS47:BV47"/>
-    <mergeCell ref="BW47:BZ47"/>
-    <mergeCell ref="AQ47:AT47"/>
-    <mergeCell ref="AU47:AX47"/>
-    <mergeCell ref="AY47:BB47"/>
-    <mergeCell ref="BC47:BF47"/>
-    <mergeCell ref="BG47:BJ47"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="O47:R47"/>
-    <mergeCell ref="S47:V47"/>
-    <mergeCell ref="W47:Z47"/>
-    <mergeCell ref="AA47:AD47"/>
-    <mergeCell ref="AE47:AH47"/>
-    <mergeCell ref="AI47:AL47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A16" r:id="rId1" xr:uid="{3202BA62-C7C1-44C7-931A-B83B37570BA9}"/>
@@ -12460,8 +13732,10 @@
     <hyperlink ref="A33" r:id="rId3" xr:uid="{19B2A9AC-A8A3-4249-B4C1-71040185C92C}"/>
     <hyperlink ref="A38" r:id="rId4" xr:uid="{F408779C-3757-49B9-84F2-A4ABC527C22E}"/>
     <hyperlink ref="A46" r:id="rId5" location="objid=4825;" display="https://www.healthypeople.gov/2020/data-search/Search-the-Data - objid=4825;" xr:uid="{6C6B7D5A-281D-491B-9320-F33FCAB2F96C}"/>
+    <hyperlink ref="A80" r:id="rId6" xr:uid="{CA9F213F-5D2E-4CAD-8868-ADF2CA06CEBD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -13371,7 +14645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58470E99-39F3-4288-B960-9BFE3E917FBC}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
template and flask route 1
</commit_message>
<xml_diff>
--- a/FinalProjectGuide.xlsx
+++ b/FinalProjectGuide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Documents\GitHub\FinalProject-MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5CB91D-0278-40F6-90EA-4DAEA467604C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B95BA84-2C80-49E3-8764-A464614808A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="7" activeTab="9" xr2:uid="{9D2C2162-F178-4CB0-81E9-DFAA2C429D49}"/>
+    <workbookView xWindow="-2415" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{9D2C2162-F178-4CB0-81E9-DFAA2C429D49}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -2154,14 +2154,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="26" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="26" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2180,28 +2202,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="26" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="26" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3122,7 +3122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CC48AC-513D-4AB1-BAEC-B7050A391FC0}">
   <dimension ref="A1:RU100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
@@ -3144,76 +3144,76 @@
       <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:489" ht="15.75" thickBot="1">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="F3" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="H3" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="I3" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="63" t="s">
+      <c r="J3" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="62" t="s">
+      <c r="K3" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="63" t="s">
+      <c r="P3" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="Q3" s="63" t="s">
+      <c r="Q3" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="63" t="s">
+      <c r="R3" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="S3" s="63" t="s">
+      <c r="S3" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="63" t="s">
+      <c r="T3" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="U3" s="62" t="s">
+      <c r="U3" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
     </row>
     <row r="4" spans="1:489" ht="30.95" customHeight="1" thickBot="1">
-      <c r="A4" s="66"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
       <c r="K4" s="4" t="s">
         <v>96</v>
       </c>
@@ -3227,11 +3227,11 @@
         <v>99</v>
       </c>
       <c r="O4" s="3"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
       <c r="U4" s="4" t="s">
         <v>96</v>
       </c>
@@ -3343,848 +3343,848 @@
     </row>
     <row r="7" spans="1:489" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:489" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A8" s="67"/>
-      <c r="B8" s="65" t="s">
+      <c r="A8" s="75"/>
+      <c r="B8" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="63" t="s">
+      <c r="E8" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="63" t="s">
+      <c r="F8" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="H8" s="65" t="s">
+      <c r="H8" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="63" t="s">
+      <c r="I8" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="J8" s="62" t="s">
+      <c r="J8" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62" t="s">
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62" t="s">
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="T8" s="62" t="s">
+      <c r="T8" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="U8" s="62"/>
-      <c r="V8" s="62"/>
-      <c r="W8" s="62" t="s">
+      <c r="U8" s="69"/>
+      <c r="V8" s="69"/>
+      <c r="W8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="X8" s="62"/>
-      <c r="Y8" s="62" t="s">
+      <c r="X8" s="69"/>
+      <c r="Y8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="Z8" s="62"/>
-      <c r="AA8" s="62" t="s">
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="AB8" s="62"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="62" t="s">
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="AE8" s="62" t="s">
+      <c r="AE8" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="AF8" s="62"/>
-      <c r="AG8" s="62"/>
-      <c r="AH8" s="62"/>
-      <c r="AI8" s="62" t="s">
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="69"/>
+      <c r="AH8" s="69"/>
+      <c r="AI8" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="AJ8" s="62"/>
-      <c r="AK8" s="62" t="s">
+      <c r="AJ8" s="69"/>
+      <c r="AK8" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="AL8" s="62"/>
-      <c r="AM8" s="62"/>
-      <c r="AN8" s="62" t="s">
+      <c r="AL8" s="69"/>
+      <c r="AM8" s="69"/>
+      <c r="AN8" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="AO8" s="62" t="s">
+      <c r="AO8" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="AP8" s="62"/>
-      <c r="AQ8" s="62"/>
-      <c r="AR8" s="62"/>
-      <c r="AS8" s="62" t="s">
+      <c r="AP8" s="69"/>
+      <c r="AQ8" s="69"/>
+      <c r="AR8" s="69"/>
+      <c r="AS8" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="AT8" s="62"/>
-      <c r="AU8" s="62"/>
-      <c r="AV8" s="62"/>
-      <c r="AW8" s="62"/>
-      <c r="AX8" s="62" t="s">
+      <c r="AT8" s="69"/>
+      <c r="AU8" s="69"/>
+      <c r="AV8" s="69"/>
+      <c r="AW8" s="69"/>
+      <c r="AX8" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="AY8" s="62"/>
-      <c r="AZ8" s="62"/>
-      <c r="BA8" s="62"/>
-      <c r="BB8" s="62" t="s">
+      <c r="AY8" s="69"/>
+      <c r="AZ8" s="69"/>
+      <c r="BA8" s="69"/>
+      <c r="BB8" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="BC8" s="62" t="s">
+      <c r="BC8" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="BD8" s="62"/>
-      <c r="BE8" s="62"/>
-      <c r="BF8" s="62" t="s">
+      <c r="BD8" s="69"/>
+      <c r="BE8" s="69"/>
+      <c r="BF8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="BG8" s="62"/>
-      <c r="BH8" s="62" t="s">
+      <c r="BG8" s="69"/>
+      <c r="BH8" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="BI8" s="62"/>
-      <c r="BJ8" s="62" t="s">
+      <c r="BI8" s="69"/>
+      <c r="BJ8" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="BK8" s="62"/>
-      <c r="BL8" s="62"/>
-      <c r="BM8" s="62" t="s">
+      <c r="BK8" s="69"/>
+      <c r="BL8" s="69"/>
+      <c r="BM8" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="BN8" s="62" t="s">
+      <c r="BN8" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="BO8" s="62"/>
-      <c r="BP8" s="62"/>
-      <c r="BQ8" s="62"/>
-      <c r="BR8" s="62" t="s">
+      <c r="BO8" s="69"/>
+      <c r="BP8" s="69"/>
+      <c r="BQ8" s="69"/>
+      <c r="BR8" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="BS8" s="62"/>
-      <c r="BT8" s="62"/>
-      <c r="BU8" s="62"/>
-      <c r="BV8" s="62"/>
-      <c r="BW8" s="62" t="s">
+      <c r="BS8" s="69"/>
+      <c r="BT8" s="69"/>
+      <c r="BU8" s="69"/>
+      <c r="BV8" s="69"/>
+      <c r="BW8" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="BX8" s="62"/>
-      <c r="BY8" s="62"/>
-      <c r="BZ8" s="62"/>
-      <c r="CA8" s="62" t="s">
+      <c r="BX8" s="69"/>
+      <c r="BY8" s="69"/>
+      <c r="BZ8" s="69"/>
+      <c r="CA8" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="CB8" s="62" t="s">
+      <c r="CB8" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="CC8" s="62"/>
-      <c r="CD8" s="62"/>
-      <c r="CE8" s="62" t="s">
+      <c r="CC8" s="69"/>
+      <c r="CD8" s="69"/>
+      <c r="CE8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="CF8" s="62"/>
-      <c r="CG8" s="62" t="s">
+      <c r="CF8" s="69"/>
+      <c r="CG8" s="69" t="s">
         <v>126</v>
       </c>
-      <c r="CH8" s="62"/>
-      <c r="CI8" s="62" t="s">
+      <c r="CH8" s="69"/>
+      <c r="CI8" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="CJ8" s="62"/>
-      <c r="CK8" s="62"/>
-      <c r="CL8" s="62" t="s">
+      <c r="CJ8" s="69"/>
+      <c r="CK8" s="69"/>
+      <c r="CL8" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="CM8" s="62" t="s">
+      <c r="CM8" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="CN8" s="62"/>
-      <c r="CO8" s="62"/>
-      <c r="CP8" s="62"/>
-      <c r="CQ8" s="62" t="s">
+      <c r="CN8" s="69"/>
+      <c r="CO8" s="69"/>
+      <c r="CP8" s="69"/>
+      <c r="CQ8" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="CR8" s="62"/>
-      <c r="CS8" s="62"/>
-      <c r="CT8" s="62"/>
-      <c r="CU8" s="62"/>
-      <c r="CV8" s="62" t="s">
+      <c r="CR8" s="69"/>
+      <c r="CS8" s="69"/>
+      <c r="CT8" s="69"/>
+      <c r="CU8" s="69"/>
+      <c r="CV8" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="CW8" s="62"/>
-      <c r="CX8" s="62"/>
-      <c r="CY8" s="62"/>
-      <c r="CZ8" s="62" t="s">
+      <c r="CW8" s="69"/>
+      <c r="CX8" s="69"/>
+      <c r="CY8" s="69"/>
+      <c r="CZ8" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="DA8" s="62" t="s">
+      <c r="DA8" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="DB8" s="62"/>
-      <c r="DC8" s="62"/>
-      <c r="DD8" s="62" t="s">
+      <c r="DB8" s="69"/>
+      <c r="DC8" s="69"/>
+      <c r="DD8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="DE8" s="62"/>
-      <c r="DF8" s="62" t="s">
+      <c r="DE8" s="69"/>
+      <c r="DF8" s="69" t="s">
         <v>131</v>
       </c>
-      <c r="DG8" s="62"/>
-      <c r="DH8" s="62" t="s">
+      <c r="DG8" s="69"/>
+      <c r="DH8" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="DI8" s="62"/>
-      <c r="DJ8" s="62"/>
-      <c r="DK8" s="62" t="s">
+      <c r="DI8" s="69"/>
+      <c r="DJ8" s="69"/>
+      <c r="DK8" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="DL8" s="62" t="s">
+      <c r="DL8" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="DM8" s="62"/>
-      <c r="DN8" s="62"/>
-      <c r="DO8" s="62"/>
-      <c r="DP8" s="62" t="s">
+      <c r="DM8" s="69"/>
+      <c r="DN8" s="69"/>
+      <c r="DO8" s="69"/>
+      <c r="DP8" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="DQ8" s="62"/>
-      <c r="DR8" s="62"/>
-      <c r="DS8" s="62"/>
-      <c r="DT8" s="62"/>
-      <c r="DU8" s="62" t="s">
+      <c r="DQ8" s="69"/>
+      <c r="DR8" s="69"/>
+      <c r="DS8" s="69"/>
+      <c r="DT8" s="69"/>
+      <c r="DU8" s="69" t="s">
         <v>134</v>
       </c>
-      <c r="DV8" s="62"/>
-      <c r="DW8" s="62"/>
-      <c r="DX8" s="62"/>
-      <c r="DY8" s="62" t="s">
+      <c r="DV8" s="69"/>
+      <c r="DW8" s="69"/>
+      <c r="DX8" s="69"/>
+      <c r="DY8" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="DZ8" s="62" t="s">
+      <c r="DZ8" s="69" t="s">
         <v>135</v>
       </c>
-      <c r="EA8" s="62"/>
-      <c r="EB8" s="62"/>
-      <c r="EC8" s="62" t="s">
+      <c r="EA8" s="69"/>
+      <c r="EB8" s="69"/>
+      <c r="EC8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="ED8" s="62"/>
-      <c r="EE8" s="62"/>
-      <c r="EF8" s="62" t="s">
+      <c r="ED8" s="69"/>
+      <c r="EE8" s="69"/>
+      <c r="EF8" s="69" t="s">
         <v>136</v>
       </c>
-      <c r="EG8" s="62"/>
-      <c r="EH8" s="62"/>
-      <c r="EI8" s="62" t="s">
+      <c r="EG8" s="69"/>
+      <c r="EH8" s="69"/>
+      <c r="EI8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="EJ8" s="62"/>
-      <c r="EK8" s="62"/>
-      <c r="EL8" s="62" t="s">
+      <c r="EJ8" s="69"/>
+      <c r="EK8" s="69"/>
+      <c r="EL8" s="69" t="s">
         <v>137</v>
       </c>
-      <c r="EM8" s="62"/>
-      <c r="EN8" s="62"/>
-      <c r="EO8" s="62" t="s">
+      <c r="EM8" s="69"/>
+      <c r="EN8" s="69"/>
+      <c r="EO8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="EP8" s="62"/>
-      <c r="EQ8" s="62"/>
-      <c r="ER8" s="62" t="s">
+      <c r="EP8" s="69"/>
+      <c r="EQ8" s="69"/>
+      <c r="ER8" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="ES8" s="62"/>
-      <c r="ET8" s="62"/>
-      <c r="EU8" s="62" t="s">
+      <c r="ES8" s="69"/>
+      <c r="ET8" s="69"/>
+      <c r="EU8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="EV8" s="62"/>
-      <c r="EW8" s="62"/>
-      <c r="EX8" s="62" t="s">
+      <c r="EV8" s="69"/>
+      <c r="EW8" s="69"/>
+      <c r="EX8" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="EY8" s="62"/>
-      <c r="EZ8" s="62"/>
-      <c r="FA8" s="62" t="s">
+      <c r="EY8" s="69"/>
+      <c r="EZ8" s="69"/>
+      <c r="FA8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="FB8" s="62"/>
-      <c r="FC8" s="62"/>
-      <c r="FD8" s="62" t="s">
+      <c r="FB8" s="69"/>
+      <c r="FC8" s="69"/>
+      <c r="FD8" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="FE8" s="62"/>
-      <c r="FF8" s="62"/>
-      <c r="FG8" s="62" t="s">
+      <c r="FE8" s="69"/>
+      <c r="FF8" s="69"/>
+      <c r="FG8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="FH8" s="62"/>
-      <c r="FI8" s="62"/>
-      <c r="FJ8" s="62" t="s">
+      <c r="FH8" s="69"/>
+      <c r="FI8" s="69"/>
+      <c r="FJ8" s="69" t="s">
         <v>141</v>
       </c>
-      <c r="FK8" s="62"/>
-      <c r="FL8" s="62"/>
-      <c r="FM8" s="62" t="s">
+      <c r="FK8" s="69"/>
+      <c r="FL8" s="69"/>
+      <c r="FM8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="FN8" s="62"/>
-      <c r="FO8" s="62"/>
-      <c r="FP8" s="62" t="s">
+      <c r="FN8" s="69"/>
+      <c r="FO8" s="69"/>
+      <c r="FP8" s="69" t="s">
         <v>142</v>
       </c>
-      <c r="FQ8" s="62"/>
-      <c r="FR8" s="62"/>
-      <c r="FS8" s="62" t="s">
+      <c r="FQ8" s="69"/>
+      <c r="FR8" s="69"/>
+      <c r="FS8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="FT8" s="62"/>
-      <c r="FU8" s="62"/>
-      <c r="FV8" s="62" t="s">
+      <c r="FT8" s="69"/>
+      <c r="FU8" s="69"/>
+      <c r="FV8" s="69" t="s">
         <v>143</v>
       </c>
-      <c r="FW8" s="62"/>
-      <c r="FX8" s="62"/>
-      <c r="FY8" s="62" t="s">
+      <c r="FW8" s="69"/>
+      <c r="FX8" s="69"/>
+      <c r="FY8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="FZ8" s="62"/>
-      <c r="GA8" s="62"/>
-      <c r="GB8" s="62" t="s">
+      <c r="FZ8" s="69"/>
+      <c r="GA8" s="69"/>
+      <c r="GB8" s="69" t="s">
         <v>144</v>
       </c>
-      <c r="GC8" s="62"/>
-      <c r="GD8" s="62"/>
-      <c r="GE8" s="62" t="s">
+      <c r="GC8" s="69"/>
+      <c r="GD8" s="69"/>
+      <c r="GE8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="GF8" s="62"/>
-      <c r="GG8" s="62"/>
-      <c r="GH8" s="62" t="s">
+      <c r="GF8" s="69"/>
+      <c r="GG8" s="69"/>
+      <c r="GH8" s="69" t="s">
         <v>145</v>
       </c>
-      <c r="GI8" s="62"/>
-      <c r="GJ8" s="62"/>
-      <c r="GK8" s="62" t="s">
+      <c r="GI8" s="69"/>
+      <c r="GJ8" s="69"/>
+      <c r="GK8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="GL8" s="62"/>
-      <c r="GM8" s="62"/>
-      <c r="GN8" s="62" t="s">
+      <c r="GL8" s="69"/>
+      <c r="GM8" s="69"/>
+      <c r="GN8" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="GO8" s="62"/>
-      <c r="GP8" s="62"/>
-      <c r="GQ8" s="62" t="s">
+      <c r="GO8" s="69"/>
+      <c r="GP8" s="69"/>
+      <c r="GQ8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="GR8" s="62"/>
-      <c r="GS8" s="62"/>
-      <c r="GT8" s="62" t="s">
+      <c r="GR8" s="69"/>
+      <c r="GS8" s="69"/>
+      <c r="GT8" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="GU8" s="62"/>
-      <c r="GV8" s="62"/>
-      <c r="GW8" s="62" t="s">
+      <c r="GU8" s="69"/>
+      <c r="GV8" s="69"/>
+      <c r="GW8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="GX8" s="62"/>
-      <c r="GY8" s="62"/>
-      <c r="GZ8" s="62" t="s">
+      <c r="GX8" s="69"/>
+      <c r="GY8" s="69"/>
+      <c r="GZ8" s="69" t="s">
         <v>148</v>
       </c>
-      <c r="HA8" s="62"/>
-      <c r="HB8" s="62"/>
-      <c r="HC8" s="62" t="s">
+      <c r="HA8" s="69"/>
+      <c r="HB8" s="69"/>
+      <c r="HC8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="HD8" s="62"/>
-      <c r="HE8" s="62"/>
-      <c r="HF8" s="62" t="s">
+      <c r="HD8" s="69"/>
+      <c r="HE8" s="69"/>
+      <c r="HF8" s="69" t="s">
         <v>149</v>
       </c>
-      <c r="HG8" s="62"/>
-      <c r="HH8" s="62"/>
-      <c r="HI8" s="62" t="s">
+      <c r="HG8" s="69"/>
+      <c r="HH8" s="69"/>
+      <c r="HI8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="HJ8" s="62"/>
-      <c r="HK8" s="62"/>
-      <c r="HL8" s="62" t="s">
+      <c r="HJ8" s="69"/>
+      <c r="HK8" s="69"/>
+      <c r="HL8" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="HM8" s="62"/>
-      <c r="HN8" s="62"/>
-      <c r="HO8" s="62" t="s">
+      <c r="HM8" s="69"/>
+      <c r="HN8" s="69"/>
+      <c r="HO8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="HP8" s="62"/>
-      <c r="HQ8" s="62"/>
-      <c r="HR8" s="62" t="s">
+      <c r="HP8" s="69"/>
+      <c r="HQ8" s="69"/>
+      <c r="HR8" s="69" t="s">
         <v>151</v>
       </c>
-      <c r="HS8" s="62"/>
-      <c r="HT8" s="62"/>
-      <c r="HU8" s="62" t="s">
+      <c r="HS8" s="69"/>
+      <c r="HT8" s="69"/>
+      <c r="HU8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="HV8" s="62"/>
-      <c r="HW8" s="62"/>
-      <c r="HX8" s="62" t="s">
+      <c r="HV8" s="69"/>
+      <c r="HW8" s="69"/>
+      <c r="HX8" s="69" t="s">
         <v>152</v>
       </c>
-      <c r="HY8" s="62"/>
-      <c r="HZ8" s="62"/>
-      <c r="IA8" s="62" t="s">
+      <c r="HY8" s="69"/>
+      <c r="HZ8" s="69"/>
+      <c r="IA8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="IB8" s="62"/>
-      <c r="IC8" s="62"/>
-      <c r="ID8" s="62" t="s">
+      <c r="IB8" s="69"/>
+      <c r="IC8" s="69"/>
+      <c r="ID8" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="IE8" s="62"/>
-      <c r="IF8" s="62"/>
-      <c r="IG8" s="62" t="s">
+      <c r="IE8" s="69"/>
+      <c r="IF8" s="69"/>
+      <c r="IG8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="IH8" s="62"/>
-      <c r="II8" s="62"/>
-      <c r="IJ8" s="62" t="s">
+      <c r="IH8" s="69"/>
+      <c r="II8" s="69"/>
+      <c r="IJ8" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="IK8" s="62"/>
-      <c r="IL8" s="62"/>
-      <c r="IM8" s="62" t="s">
+      <c r="IK8" s="69"/>
+      <c r="IL8" s="69"/>
+      <c r="IM8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="IN8" s="62"/>
-      <c r="IO8" s="62"/>
-      <c r="IP8" s="62" t="s">
+      <c r="IN8" s="69"/>
+      <c r="IO8" s="69"/>
+      <c r="IP8" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="IQ8" s="62"/>
-      <c r="IR8" s="62"/>
-      <c r="IS8" s="62" t="s">
+      <c r="IQ8" s="69"/>
+      <c r="IR8" s="69"/>
+      <c r="IS8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="IT8" s="62"/>
-      <c r="IU8" s="62"/>
-      <c r="IV8" s="62" t="s">
+      <c r="IT8" s="69"/>
+      <c r="IU8" s="69"/>
+      <c r="IV8" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="IW8" s="62"/>
-      <c r="IX8" s="62"/>
-      <c r="IY8" s="62" t="s">
+      <c r="IW8" s="69"/>
+      <c r="IX8" s="69"/>
+      <c r="IY8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="IZ8" s="62"/>
-      <c r="JA8" s="62"/>
-      <c r="JB8" s="62" t="s">
+      <c r="IZ8" s="69"/>
+      <c r="JA8" s="69"/>
+      <c r="JB8" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="JC8" s="62"/>
-      <c r="JD8" s="62"/>
-      <c r="JE8" s="62" t="s">
+      <c r="JC8" s="69"/>
+      <c r="JD8" s="69"/>
+      <c r="JE8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="JF8" s="62"/>
-      <c r="JG8" s="62"/>
-      <c r="JH8" s="62" t="s">
+      <c r="JF8" s="69"/>
+      <c r="JG8" s="69"/>
+      <c r="JH8" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="JI8" s="62"/>
-      <c r="JJ8" s="62"/>
-      <c r="JK8" s="62" t="s">
+      <c r="JI8" s="69"/>
+      <c r="JJ8" s="69"/>
+      <c r="JK8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="JL8" s="62"/>
-      <c r="JM8" s="62"/>
-      <c r="JN8" s="62" t="s">
+      <c r="JL8" s="69"/>
+      <c r="JM8" s="69"/>
+      <c r="JN8" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="JO8" s="62"/>
-      <c r="JP8" s="62"/>
-      <c r="JQ8" s="62" t="s">
+      <c r="JO8" s="69"/>
+      <c r="JP8" s="69"/>
+      <c r="JQ8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="JR8" s="62"/>
-      <c r="JS8" s="62"/>
-      <c r="JT8" s="62" t="s">
+      <c r="JR8" s="69"/>
+      <c r="JS8" s="69"/>
+      <c r="JT8" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="JU8" s="62"/>
-      <c r="JV8" s="62"/>
-      <c r="JW8" s="62" t="s">
+      <c r="JU8" s="69"/>
+      <c r="JV8" s="69"/>
+      <c r="JW8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="JX8" s="62"/>
-      <c r="JY8" s="62"/>
-      <c r="JZ8" s="62" t="s">
+      <c r="JX8" s="69"/>
+      <c r="JY8" s="69"/>
+      <c r="JZ8" s="69" t="s">
         <v>161</v>
       </c>
-      <c r="KA8" s="62"/>
-      <c r="KB8" s="62"/>
-      <c r="KC8" s="62" t="s">
+      <c r="KA8" s="69"/>
+      <c r="KB8" s="69"/>
+      <c r="KC8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="KD8" s="62"/>
-      <c r="KE8" s="62"/>
-      <c r="KF8" s="62" t="s">
+      <c r="KD8" s="69"/>
+      <c r="KE8" s="69"/>
+      <c r="KF8" s="69" t="s">
         <v>162</v>
       </c>
-      <c r="KG8" s="62"/>
-      <c r="KH8" s="62"/>
-      <c r="KI8" s="62" t="s">
+      <c r="KG8" s="69"/>
+      <c r="KH8" s="69"/>
+      <c r="KI8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="KJ8" s="62"/>
-      <c r="KK8" s="62"/>
-      <c r="KL8" s="62" t="s">
+      <c r="KJ8" s="69"/>
+      <c r="KK8" s="69"/>
+      <c r="KL8" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="KM8" s="62"/>
-      <c r="KN8" s="62"/>
-      <c r="KO8" s="62" t="s">
+      <c r="KM8" s="69"/>
+      <c r="KN8" s="69"/>
+      <c r="KO8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="KP8" s="62"/>
-      <c r="KQ8" s="62"/>
-      <c r="KR8" s="62" t="s">
+      <c r="KP8" s="69"/>
+      <c r="KQ8" s="69"/>
+      <c r="KR8" s="69" t="s">
         <v>164</v>
       </c>
-      <c r="KS8" s="62"/>
-      <c r="KT8" s="62"/>
-      <c r="KU8" s="62" t="s">
+      <c r="KS8" s="69"/>
+      <c r="KT8" s="69"/>
+      <c r="KU8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="KV8" s="62"/>
-      <c r="KW8" s="62"/>
-      <c r="KX8" s="62" t="s">
+      <c r="KV8" s="69"/>
+      <c r="KW8" s="69"/>
+      <c r="KX8" s="69" t="s">
         <v>165</v>
       </c>
-      <c r="KY8" s="62"/>
-      <c r="KZ8" s="62"/>
-      <c r="LA8" s="62" t="s">
+      <c r="KY8" s="69"/>
+      <c r="KZ8" s="69"/>
+      <c r="LA8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="LB8" s="62"/>
-      <c r="LC8" s="62"/>
-      <c r="LD8" s="62" t="s">
+      <c r="LB8" s="69"/>
+      <c r="LC8" s="69"/>
+      <c r="LD8" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="LE8" s="62"/>
-      <c r="LF8" s="62"/>
-      <c r="LG8" s="62" t="s">
+      <c r="LE8" s="69"/>
+      <c r="LF8" s="69"/>
+      <c r="LG8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="LH8" s="62"/>
-      <c r="LI8" s="62"/>
-      <c r="LJ8" s="62" t="s">
+      <c r="LH8" s="69"/>
+      <c r="LI8" s="69"/>
+      <c r="LJ8" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="LK8" s="62"/>
-      <c r="LL8" s="62"/>
-      <c r="LM8" s="62" t="s">
+      <c r="LK8" s="69"/>
+      <c r="LL8" s="69"/>
+      <c r="LM8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="LN8" s="62"/>
-      <c r="LO8" s="62"/>
-      <c r="LP8" s="62" t="s">
+      <c r="LN8" s="69"/>
+      <c r="LO8" s="69"/>
+      <c r="LP8" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="LQ8" s="62"/>
-      <c r="LR8" s="62"/>
-      <c r="LS8" s="62" t="s">
+      <c r="LQ8" s="69"/>
+      <c r="LR8" s="69"/>
+      <c r="LS8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="LT8" s="62"/>
-      <c r="LU8" s="62"/>
-      <c r="LV8" s="62" t="s">
+      <c r="LT8" s="69"/>
+      <c r="LU8" s="69"/>
+      <c r="LV8" s="69" t="s">
         <v>169</v>
       </c>
-      <c r="LW8" s="62"/>
-      <c r="LX8" s="62"/>
-      <c r="LY8" s="62" t="s">
+      <c r="LW8" s="69"/>
+      <c r="LX8" s="69"/>
+      <c r="LY8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="LZ8" s="62"/>
-      <c r="MA8" s="62"/>
-      <c r="MB8" s="62" t="s">
+      <c r="LZ8" s="69"/>
+      <c r="MA8" s="69"/>
+      <c r="MB8" s="69" t="s">
         <v>170</v>
       </c>
-      <c r="MC8" s="62"/>
-      <c r="MD8" s="62"/>
-      <c r="ME8" s="62" t="s">
+      <c r="MC8" s="69"/>
+      <c r="MD8" s="69"/>
+      <c r="ME8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="MF8" s="62"/>
-      <c r="MG8" s="62"/>
-      <c r="MH8" s="62" t="s">
+      <c r="MF8" s="69"/>
+      <c r="MG8" s="69"/>
+      <c r="MH8" s="69" t="s">
         <v>171</v>
       </c>
-      <c r="MI8" s="62"/>
-      <c r="MJ8" s="62"/>
-      <c r="MK8" s="62" t="s">
+      <c r="MI8" s="69"/>
+      <c r="MJ8" s="69"/>
+      <c r="MK8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="ML8" s="62"/>
-      <c r="MM8" s="62"/>
-      <c r="MN8" s="62" t="s">
+      <c r="ML8" s="69"/>
+      <c r="MM8" s="69"/>
+      <c r="MN8" s="69" t="s">
         <v>172</v>
       </c>
-      <c r="MO8" s="62"/>
-      <c r="MP8" s="62"/>
-      <c r="MQ8" s="62" t="s">
+      <c r="MO8" s="69"/>
+      <c r="MP8" s="69"/>
+      <c r="MQ8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="MR8" s="62"/>
-      <c r="MS8" s="62"/>
-      <c r="MT8" s="62" t="s">
+      <c r="MR8" s="69"/>
+      <c r="MS8" s="69"/>
+      <c r="MT8" s="69" t="s">
         <v>173</v>
       </c>
-      <c r="MU8" s="62"/>
-      <c r="MV8" s="62"/>
-      <c r="MW8" s="62" t="s">
+      <c r="MU8" s="69"/>
+      <c r="MV8" s="69"/>
+      <c r="MW8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="MX8" s="62"/>
-      <c r="MY8" s="62"/>
-      <c r="MZ8" s="62" t="s">
+      <c r="MX8" s="69"/>
+      <c r="MY8" s="69"/>
+      <c r="MZ8" s="69" t="s">
         <v>174</v>
       </c>
-      <c r="NA8" s="62"/>
-      <c r="NB8" s="62"/>
-      <c r="NC8" s="62" t="s">
+      <c r="NA8" s="69"/>
+      <c r="NB8" s="69"/>
+      <c r="NC8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="ND8" s="62"/>
-      <c r="NE8" s="62"/>
-      <c r="NF8" s="62" t="s">
+      <c r="ND8" s="69"/>
+      <c r="NE8" s="69"/>
+      <c r="NF8" s="69" t="s">
         <v>175</v>
       </c>
-      <c r="NG8" s="62"/>
-      <c r="NH8" s="62"/>
-      <c r="NI8" s="62" t="s">
+      <c r="NG8" s="69"/>
+      <c r="NH8" s="69"/>
+      <c r="NI8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="NJ8" s="62"/>
-      <c r="NK8" s="62"/>
-      <c r="NL8" s="62" t="s">
+      <c r="NJ8" s="69"/>
+      <c r="NK8" s="69"/>
+      <c r="NL8" s="69" t="s">
         <v>176</v>
       </c>
-      <c r="NM8" s="62"/>
-      <c r="NN8" s="62"/>
-      <c r="NO8" s="62" t="s">
+      <c r="NM8" s="69"/>
+      <c r="NN8" s="69"/>
+      <c r="NO8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="NP8" s="62"/>
-      <c r="NQ8" s="62"/>
-      <c r="NR8" s="62" t="s">
+      <c r="NP8" s="69"/>
+      <c r="NQ8" s="69"/>
+      <c r="NR8" s="69" t="s">
         <v>177</v>
       </c>
-      <c r="NS8" s="62"/>
-      <c r="NT8" s="62"/>
-      <c r="NU8" s="62" t="s">
+      <c r="NS8" s="69"/>
+      <c r="NT8" s="69"/>
+      <c r="NU8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="NV8" s="62"/>
-      <c r="NW8" s="62"/>
-      <c r="NX8" s="62" t="s">
+      <c r="NV8" s="69"/>
+      <c r="NW8" s="69"/>
+      <c r="NX8" s="69" t="s">
         <v>178</v>
       </c>
-      <c r="NY8" s="62"/>
-      <c r="NZ8" s="62"/>
-      <c r="OA8" s="62" t="s">
+      <c r="NY8" s="69"/>
+      <c r="NZ8" s="69"/>
+      <c r="OA8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="OB8" s="62"/>
-      <c r="OC8" s="62"/>
-      <c r="OD8" s="62" t="s">
+      <c r="OB8" s="69"/>
+      <c r="OC8" s="69"/>
+      <c r="OD8" s="69" t="s">
         <v>179</v>
       </c>
-      <c r="OE8" s="62"/>
-      <c r="OF8" s="62"/>
-      <c r="OG8" s="62" t="s">
+      <c r="OE8" s="69"/>
+      <c r="OF8" s="69"/>
+      <c r="OG8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="OH8" s="62"/>
-      <c r="OI8" s="62"/>
-      <c r="OJ8" s="62" t="s">
+      <c r="OH8" s="69"/>
+      <c r="OI8" s="69"/>
+      <c r="OJ8" s="69" t="s">
         <v>180</v>
       </c>
-      <c r="OK8" s="62"/>
-      <c r="OL8" s="62"/>
-      <c r="OM8" s="62" t="s">
+      <c r="OK8" s="69"/>
+      <c r="OL8" s="69"/>
+      <c r="OM8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="ON8" s="62"/>
-      <c r="OO8" s="62"/>
-      <c r="OP8" s="62" t="s">
+      <c r="ON8" s="69"/>
+      <c r="OO8" s="69"/>
+      <c r="OP8" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="OQ8" s="62"/>
-      <c r="OR8" s="62"/>
-      <c r="OS8" s="62" t="s">
+      <c r="OQ8" s="69"/>
+      <c r="OR8" s="69"/>
+      <c r="OS8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="OT8" s="62"/>
-      <c r="OU8" s="62"/>
-      <c r="OV8" s="62" t="s">
+      <c r="OT8" s="69"/>
+      <c r="OU8" s="69"/>
+      <c r="OV8" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="OW8" s="62"/>
-      <c r="OX8" s="62"/>
-      <c r="OY8" s="62" t="s">
+      <c r="OW8" s="69"/>
+      <c r="OX8" s="69"/>
+      <c r="OY8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="OZ8" s="62"/>
-      <c r="PA8" s="62"/>
-      <c r="PB8" s="62" t="s">
+      <c r="OZ8" s="69"/>
+      <c r="PA8" s="69"/>
+      <c r="PB8" s="69" t="s">
         <v>183</v>
       </c>
-      <c r="PC8" s="62"/>
-      <c r="PD8" s="62"/>
-      <c r="PE8" s="62" t="s">
+      <c r="PC8" s="69"/>
+      <c r="PD8" s="69"/>
+      <c r="PE8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="PF8" s="62"/>
-      <c r="PG8" s="62"/>
-      <c r="PH8" s="62" t="s">
+      <c r="PF8" s="69"/>
+      <c r="PG8" s="69"/>
+      <c r="PH8" s="69" t="s">
         <v>184</v>
       </c>
-      <c r="PI8" s="62"/>
-      <c r="PJ8" s="62"/>
-      <c r="PK8" s="62" t="s">
+      <c r="PI8" s="69"/>
+      <c r="PJ8" s="69"/>
+      <c r="PK8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="PL8" s="62"/>
-      <c r="PM8" s="62"/>
-      <c r="PN8" s="62" t="s">
+      <c r="PL8" s="69"/>
+      <c r="PM8" s="69"/>
+      <c r="PN8" s="69" t="s">
         <v>185</v>
       </c>
-      <c r="PO8" s="62"/>
-      <c r="PP8" s="62"/>
-      <c r="PQ8" s="62" t="s">
+      <c r="PO8" s="69"/>
+      <c r="PP8" s="69"/>
+      <c r="PQ8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="PR8" s="62"/>
-      <c r="PS8" s="62"/>
-      <c r="PT8" s="62" t="s">
+      <c r="PR8" s="69"/>
+      <c r="PS8" s="69"/>
+      <c r="PT8" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="PU8" s="62"/>
-      <c r="PV8" s="62"/>
-      <c r="PW8" s="62" t="s">
+      <c r="PU8" s="69"/>
+      <c r="PV8" s="69"/>
+      <c r="PW8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="PX8" s="62"/>
-      <c r="PY8" s="62"/>
-      <c r="PZ8" s="62" t="s">
+      <c r="PX8" s="69"/>
+      <c r="PY8" s="69"/>
+      <c r="PZ8" s="69" t="s">
         <v>187</v>
       </c>
-      <c r="QA8" s="62"/>
-      <c r="QB8" s="62"/>
-      <c r="QC8" s="62" t="s">
+      <c r="QA8" s="69"/>
+      <c r="QB8" s="69"/>
+      <c r="QC8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="QD8" s="62"/>
-      <c r="QE8" s="62"/>
-      <c r="QF8" s="62" t="s">
+      <c r="QD8" s="69"/>
+      <c r="QE8" s="69"/>
+      <c r="QF8" s="69" t="s">
         <v>188</v>
       </c>
-      <c r="QG8" s="62"/>
-      <c r="QH8" s="62"/>
-      <c r="QI8" s="62" t="s">
+      <c r="QG8" s="69"/>
+      <c r="QH8" s="69"/>
+      <c r="QI8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="QJ8" s="62"/>
-      <c r="QK8" s="62"/>
-      <c r="QL8" s="62" t="s">
+      <c r="QJ8" s="69"/>
+      <c r="QK8" s="69"/>
+      <c r="QL8" s="69" t="s">
         <v>189</v>
       </c>
-      <c r="QM8" s="62"/>
-      <c r="QN8" s="62"/>
-      <c r="QO8" s="62" t="s">
+      <c r="QM8" s="69"/>
+      <c r="QN8" s="69"/>
+      <c r="QO8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="QP8" s="62"/>
-      <c r="QQ8" s="62"/>
-      <c r="QR8" s="62" t="s">
+      <c r="QP8" s="69"/>
+      <c r="QQ8" s="69"/>
+      <c r="QR8" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="QS8" s="62"/>
-      <c r="QT8" s="62"/>
-      <c r="QU8" s="62" t="s">
+      <c r="QS8" s="69"/>
+      <c r="QT8" s="69"/>
+      <c r="QU8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="QV8" s="62"/>
-      <c r="QW8" s="62"/>
-      <c r="QX8" s="62" t="s">
+      <c r="QV8" s="69"/>
+      <c r="QW8" s="69"/>
+      <c r="QX8" s="69" t="s">
         <v>191</v>
       </c>
-      <c r="QY8" s="62"/>
-      <c r="QZ8" s="62"/>
-      <c r="RA8" s="62" t="s">
+      <c r="QY8" s="69"/>
+      <c r="QZ8" s="69"/>
+      <c r="RA8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="RB8" s="62"/>
-      <c r="RC8" s="62"/>
-      <c r="RD8" s="62" t="s">
+      <c r="RB8" s="69"/>
+      <c r="RC8" s="69"/>
+      <c r="RD8" s="69" t="s">
         <v>192</v>
       </c>
-      <c r="RE8" s="62"/>
-      <c r="RF8" s="62"/>
-      <c r="RG8" s="62" t="s">
+      <c r="RE8" s="69"/>
+      <c r="RF8" s="69"/>
+      <c r="RG8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="RH8" s="62"/>
-      <c r="RI8" s="62"/>
-      <c r="RJ8" s="62" t="s">
+      <c r="RH8" s="69"/>
+      <c r="RI8" s="69"/>
+      <c r="RJ8" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="RK8" s="62"/>
-      <c r="RL8" s="62"/>
-      <c r="RM8" s="62" t="s">
+      <c r="RK8" s="69"/>
+      <c r="RL8" s="69"/>
+      <c r="RM8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="RN8" s="62"/>
-      <c r="RO8" s="62"/>
-      <c r="RP8" s="62" t="s">
+      <c r="RN8" s="69"/>
+      <c r="RO8" s="69"/>
+      <c r="RP8" s="69" t="s">
         <v>194</v>
       </c>
-      <c r="RQ8" s="62"/>
-      <c r="RR8" s="62"/>
-      <c r="RS8" s="62" t="s">
+      <c r="RQ8" s="69"/>
+      <c r="RR8" s="69"/>
+      <c r="RS8" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="RT8" s="62"/>
-      <c r="RU8" s="62"/>
+      <c r="RT8" s="69"/>
+      <c r="RU8" s="69"/>
     </row>
     <row r="9" spans="1:489" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A9" s="68"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="64"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="72"/>
       <c r="J9" s="4" t="s">
         <v>96</v>
       </c>
@@ -7012,39 +7012,39 @@
       </c>
     </row>
     <row r="34" spans="1:78" ht="15" customHeight="1">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="70" t="s">
         <v>243</v>
       </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
     </row>
     <row r="35" spans="1:78">
-      <c r="A35" s="69"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="69"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
     </row>
     <row r="36" spans="1:78" ht="78.75" customHeight="1">
-      <c r="A36" s="69"/>
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="69"/>
+      <c r="A36" s="70"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
     </row>
     <row r="38" spans="1:78">
       <c r="A38" s="1" t="s">
@@ -7372,120 +7372,120 @@
     <row r="47" spans="1:78">
       <c r="A47" s="43"/>
       <c r="B47" s="45"/>
-      <c r="C47" s="70">
+      <c r="C47" s="67">
         <v>1998</v>
       </c>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="70">
+      <c r="D47" s="68"/>
+      <c r="E47" s="68"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="67">
         <v>1999</v>
       </c>
-      <c r="H47" s="71"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="71"/>
-      <c r="K47" s="70">
+      <c r="H47" s="68"/>
+      <c r="I47" s="68"/>
+      <c r="J47" s="68"/>
+      <c r="K47" s="67">
         <v>2000</v>
       </c>
-      <c r="L47" s="71"/>
-      <c r="M47" s="71"/>
-      <c r="N47" s="71"/>
-      <c r="O47" s="70">
+      <c r="L47" s="68"/>
+      <c r="M47" s="68"/>
+      <c r="N47" s="68"/>
+      <c r="O47" s="67">
         <v>2001</v>
       </c>
-      <c r="P47" s="71"/>
-      <c r="Q47" s="71"/>
-      <c r="R47" s="71"/>
-      <c r="S47" s="70">
+      <c r="P47" s="68"/>
+      <c r="Q47" s="68"/>
+      <c r="R47" s="68"/>
+      <c r="S47" s="67">
         <v>2002</v>
       </c>
-      <c r="T47" s="71"/>
-      <c r="U47" s="71"/>
-      <c r="V47" s="71"/>
-      <c r="W47" s="70">
+      <c r="T47" s="68"/>
+      <c r="U47" s="68"/>
+      <c r="V47" s="68"/>
+      <c r="W47" s="67">
         <v>2003</v>
       </c>
-      <c r="X47" s="71"/>
-      <c r="Y47" s="71"/>
-      <c r="Z47" s="71"/>
-      <c r="AA47" s="70">
+      <c r="X47" s="68"/>
+      <c r="Y47" s="68"/>
+      <c r="Z47" s="68"/>
+      <c r="AA47" s="67">
         <v>2004</v>
       </c>
-      <c r="AB47" s="71"/>
-      <c r="AC47" s="71"/>
-      <c r="AD47" s="71"/>
-      <c r="AE47" s="70">
+      <c r="AB47" s="68"/>
+      <c r="AC47" s="68"/>
+      <c r="AD47" s="68"/>
+      <c r="AE47" s="67">
         <v>2005</v>
       </c>
-      <c r="AF47" s="71"/>
-      <c r="AG47" s="71"/>
-      <c r="AH47" s="71"/>
-      <c r="AI47" s="70">
+      <c r="AF47" s="68"/>
+      <c r="AG47" s="68"/>
+      <c r="AH47" s="68"/>
+      <c r="AI47" s="67">
         <v>2006</v>
       </c>
-      <c r="AJ47" s="71"/>
-      <c r="AK47" s="71"/>
-      <c r="AL47" s="71"/>
-      <c r="AM47" s="70">
+      <c r="AJ47" s="68"/>
+      <c r="AK47" s="68"/>
+      <c r="AL47" s="68"/>
+      <c r="AM47" s="67">
         <v>2007</v>
       </c>
-      <c r="AN47" s="71"/>
-      <c r="AO47" s="71"/>
-      <c r="AP47" s="71"/>
-      <c r="AQ47" s="70">
+      <c r="AN47" s="68"/>
+      <c r="AO47" s="68"/>
+      <c r="AP47" s="68"/>
+      <c r="AQ47" s="67">
         <v>2008</v>
       </c>
-      <c r="AR47" s="71"/>
-      <c r="AS47" s="71"/>
-      <c r="AT47" s="71"/>
-      <c r="AU47" s="70">
+      <c r="AR47" s="68"/>
+      <c r="AS47" s="68"/>
+      <c r="AT47" s="68"/>
+      <c r="AU47" s="67">
         <v>2009</v>
       </c>
-      <c r="AV47" s="71"/>
-      <c r="AW47" s="71"/>
-      <c r="AX47" s="71"/>
-      <c r="AY47" s="70">
+      <c r="AV47" s="68"/>
+      <c r="AW47" s="68"/>
+      <c r="AX47" s="68"/>
+      <c r="AY47" s="67">
         <v>2010</v>
       </c>
-      <c r="AZ47" s="71"/>
-      <c r="BA47" s="71"/>
-      <c r="BB47" s="71"/>
-      <c r="BC47" s="70">
+      <c r="AZ47" s="68"/>
+      <c r="BA47" s="68"/>
+      <c r="BB47" s="68"/>
+      <c r="BC47" s="67">
         <v>2011</v>
       </c>
-      <c r="BD47" s="71"/>
-      <c r="BE47" s="71"/>
-      <c r="BF47" s="71"/>
-      <c r="BG47" s="70">
+      <c r="BD47" s="68"/>
+      <c r="BE47" s="68"/>
+      <c r="BF47" s="68"/>
+      <c r="BG47" s="67">
         <v>2012</v>
       </c>
-      <c r="BH47" s="71"/>
-      <c r="BI47" s="71"/>
-      <c r="BJ47" s="71"/>
-      <c r="BK47" s="70">
+      <c r="BH47" s="68"/>
+      <c r="BI47" s="68"/>
+      <c r="BJ47" s="68"/>
+      <c r="BK47" s="67">
         <v>2013</v>
       </c>
-      <c r="BL47" s="71"/>
-      <c r="BM47" s="71"/>
-      <c r="BN47" s="71"/>
-      <c r="BO47" s="70">
+      <c r="BL47" s="68"/>
+      <c r="BM47" s="68"/>
+      <c r="BN47" s="68"/>
+      <c r="BO47" s="67">
         <v>2014</v>
       </c>
-      <c r="BP47" s="71"/>
-      <c r="BQ47" s="71"/>
-      <c r="BR47" s="71"/>
-      <c r="BS47" s="70">
+      <c r="BP47" s="68"/>
+      <c r="BQ47" s="68"/>
+      <c r="BR47" s="68"/>
+      <c r="BS47" s="67">
         <v>2015</v>
       </c>
-      <c r="BT47" s="71"/>
-      <c r="BU47" s="71"/>
-      <c r="BV47" s="71"/>
-      <c r="BW47" s="70">
+      <c r="BT47" s="68"/>
+      <c r="BU47" s="68"/>
+      <c r="BV47" s="68"/>
+      <c r="BW47" s="67">
         <v>2016</v>
       </c>
-      <c r="BX47" s="71"/>
-      <c r="BY47" s="71"/>
-      <c r="BZ47" s="71"/>
+      <c r="BX47" s="68"/>
+      <c r="BY47" s="68"/>
+      <c r="BZ47" s="68"/>
     </row>
     <row r="48" spans="1:78">
       <c r="A48" s="44" t="s">
@@ -12541,699 +12541,699 @@
       </c>
     </row>
     <row r="82" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A82" s="72" t="s">
+      <c r="A82" s="60" t="s">
         <v>461</v>
       </c>
-      <c r="B82" s="72" t="s">
+      <c r="B82" s="60" t="s">
         <v>462</v>
       </c>
-      <c r="C82" s="72" t="s">
+      <c r="C82" s="60" t="s">
         <v>463</v>
       </c>
-      <c r="D82" s="72" t="s">
+      <c r="D82" s="60" t="s">
         <v>464</v>
       </c>
-      <c r="E82" s="72" t="s">
+      <c r="E82" s="60" t="s">
         <v>465</v>
       </c>
-      <c r="F82" s="72" t="s">
+      <c r="F82" s="60" t="s">
         <v>466</v>
       </c>
-      <c r="G82" s="72" t="s">
+      <c r="G82" s="60" t="s">
         <v>467</v>
       </c>
-      <c r="H82" s="72" t="s">
+      <c r="H82" s="60" t="s">
         <v>468</v>
       </c>
-      <c r="I82" s="72" t="s">
+      <c r="I82" s="60" t="s">
         <v>469</v>
       </c>
-      <c r="J82" s="72" t="s">
+      <c r="J82" s="60" t="s">
         <v>470</v>
       </c>
-      <c r="K82" s="72" t="s">
+      <c r="K82" s="60" t="s">
         <v>471</v>
       </c>
-      <c r="L82" s="72" t="s">
+      <c r="L82" s="60" t="s">
         <v>472</v>
       </c>
-      <c r="M82" s="72" t="s">
+      <c r="M82" s="60" t="s">
         <v>473</v>
       </c>
-      <c r="N82" s="72" t="s">
+      <c r="N82" s="60" t="s">
         <v>474</v>
       </c>
-      <c r="O82" s="72" t="s">
+      <c r="O82" s="60" t="s">
         <v>475</v>
       </c>
-      <c r="P82" s="72" t="s">
+      <c r="P82" s="60" t="s">
         <v>476</v>
       </c>
-      <c r="Q82" s="72" t="s">
+      <c r="Q82" s="60" t="s">
         <v>477</v>
       </c>
-      <c r="R82" s="72" t="s">
+      <c r="R82" s="60" t="s">
         <v>478</v>
       </c>
-      <c r="S82" s="72" t="s">
+      <c r="S82" s="60" t="s">
         <v>479</v>
       </c>
-      <c r="T82" s="72" t="s">
+      <c r="T82" s="60" t="s">
         <v>480</v>
       </c>
-      <c r="U82" s="72" t="s">
+      <c r="U82" s="60" t="s">
         <v>481</v>
       </c>
-      <c r="V82" s="72" t="s">
+      <c r="V82" s="60" t="s">
         <v>482</v>
       </c>
-      <c r="W82" s="72" t="s">
+      <c r="W82" s="60" t="s">
         <v>483</v>
       </c>
       <c r="X82" s="25"/>
     </row>
     <row r="83" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A83" s="73">
+      <c r="A83" s="61">
         <v>3</v>
       </c>
-      <c r="B83" s="73">
+      <c r="B83" s="61">
         <v>35</v>
       </c>
-      <c r="C83" s="73">
+      <c r="C83" s="61">
         <v>25</v>
       </c>
-      <c r="D83" s="73">
+      <c r="D83" s="61">
         <v>29.368358910000001</v>
       </c>
-      <c r="E83" s="73">
+      <c r="E83" s="61">
         <v>0</v>
       </c>
-      <c r="F83" s="73">
+      <c r="F83" s="61">
         <v>1</v>
       </c>
-      <c r="G83" s="73">
+      <c r="G83" s="61">
         <v>1</v>
       </c>
-      <c r="H83" s="73">
+      <c r="H83" s="61">
         <v>1</v>
       </c>
-      <c r="I83" s="73">
+      <c r="I83" s="61">
         <v>20</v>
       </c>
-      <c r="J83" s="73">
+      <c r="J83" s="61">
         <v>0</v>
       </c>
-      <c r="K83" s="73">
+      <c r="K83" s="61">
         <v>2.0698400000000001E-4</v>
       </c>
-      <c r="L83" s="73">
+      <c r="L83" s="61">
         <v>6.5446134000000003E-2</v>
       </c>
-      <c r="M83" s="74">
+      <c r="M83" s="62">
         <v>5.0300000000000001E-6</v>
       </c>
-      <c r="N83" s="74">
+      <c r="N83" s="62">
         <v>6.8999999999999997E-5</v>
       </c>
-      <c r="O83" s="73">
+      <c r="O83" s="61">
         <v>3.5213380000000002E-3</v>
       </c>
-      <c r="P83" s="73">
+      <c r="P83" s="61">
         <v>0</v>
       </c>
-      <c r="Q83" s="73">
+      <c r="Q83" s="61">
         <v>0</v>
       </c>
-      <c r="R83" s="73">
+      <c r="R83" s="61">
         <v>0</v>
       </c>
-      <c r="S83" s="73">
+      <c r="S83" s="61">
         <v>0</v>
       </c>
-      <c r="T83" s="73">
+      <c r="T83" s="61">
         <v>0</v>
       </c>
-      <c r="U83" s="73">
+      <c r="U83" s="61">
         <v>0.93070390800000002</v>
       </c>
-      <c r="V83" s="73">
+      <c r="V83" s="61">
         <v>0</v>
       </c>
-      <c r="W83" s="74">
+      <c r="W83" s="62">
         <v>4.7599999999999998E-5</v>
       </c>
     </row>
     <row r="84" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A84" s="75">
+      <c r="A84" s="63">
         <v>3</v>
       </c>
-      <c r="B84" s="75">
+      <c r="B84" s="63">
         <v>36</v>
       </c>
-      <c r="C84" s="75">
+      <c r="C84" s="63">
         <v>25</v>
       </c>
-      <c r="D84" s="75">
+      <c r="D84" s="63">
         <v>29.48642267</v>
       </c>
-      <c r="E84" s="75">
+      <c r="E84" s="63">
         <v>0</v>
       </c>
-      <c r="F84" s="75">
+      <c r="F84" s="63">
         <v>1</v>
       </c>
-      <c r="G84" s="75">
+      <c r="G84" s="63">
         <v>1</v>
       </c>
-      <c r="H84" s="75">
+      <c r="H84" s="63">
         <v>1</v>
       </c>
-      <c r="I84" s="75">
+      <c r="I84" s="63">
         <v>20</v>
       </c>
-      <c r="J84" s="75">
+      <c r="J84" s="63">
         <v>0</v>
       </c>
-      <c r="K84" s="75">
+      <c r="K84" s="63">
         <v>1.8755900000000001E-4</v>
       </c>
-      <c r="L84" s="75">
+      <c r="L84" s="63">
         <v>0.13525103799999999</v>
       </c>
-      <c r="M84" s="76">
+      <c r="M84" s="64">
         <v>7.7800000000000001E-7</v>
       </c>
-      <c r="N84" s="76">
+      <c r="N84" s="64">
         <v>6.2500000000000001E-5</v>
       </c>
-      <c r="O84" s="75">
+      <c r="O84" s="63">
         <v>2.9583801E-2</v>
       </c>
-      <c r="P84" s="75">
+      <c r="P84" s="63">
         <v>0</v>
       </c>
-      <c r="Q84" s="75">
+      <c r="Q84" s="63">
         <v>0</v>
       </c>
-      <c r="R84" s="75">
+      <c r="R84" s="63">
         <v>0</v>
       </c>
-      <c r="S84" s="75">
+      <c r="S84" s="63">
         <v>0</v>
       </c>
-      <c r="T84" s="75">
+      <c r="T84" s="63">
         <v>0</v>
       </c>
-      <c r="U84" s="75">
+      <c r="U84" s="63">
         <v>0.83486074899999996</v>
       </c>
-      <c r="V84" s="75">
+      <c r="V84" s="63">
         <v>0</v>
       </c>
-      <c r="W84" s="76">
+      <c r="W84" s="64">
         <v>5.3600000000000002E-5</v>
       </c>
     </row>
     <row r="85" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A85" s="73">
+      <c r="A85" s="61">
         <v>3</v>
       </c>
-      <c r="B85" s="73">
+      <c r="B85" s="61">
         <v>37</v>
       </c>
-      <c r="C85" s="73">
+      <c r="C85" s="61">
         <v>25</v>
       </c>
-      <c r="D85" s="73">
+      <c r="D85" s="61">
         <v>29.604486420000001</v>
       </c>
-      <c r="E85" s="73">
+      <c r="E85" s="61">
         <v>0</v>
       </c>
-      <c r="F85" s="73">
+      <c r="F85" s="61">
         <v>1</v>
       </c>
-      <c r="G85" s="73">
+      <c r="G85" s="61">
         <v>1</v>
       </c>
-      <c r="H85" s="73">
+      <c r="H85" s="61">
         <v>1</v>
       </c>
-      <c r="I85" s="73">
+      <c r="I85" s="61">
         <v>20</v>
       </c>
-      <c r="J85" s="73">
+      <c r="J85" s="61">
         <v>0</v>
       </c>
-      <c r="K85" s="73">
+      <c r="K85" s="61">
         <v>1.66379E-4</v>
       </c>
-      <c r="L85" s="73">
+      <c r="L85" s="61">
         <v>0.16778886700000001</v>
       </c>
-      <c r="M85" s="73">
+      <c r="M85" s="61">
         <v>0</v>
       </c>
-      <c r="N85" s="74">
+      <c r="N85" s="62">
         <v>5.5399999999999998E-5</v>
       </c>
-      <c r="O85" s="73">
+      <c r="O85" s="61">
         <v>4.1817958000000002E-2</v>
       </c>
-      <c r="P85" s="73">
+      <c r="P85" s="61">
         <v>0</v>
       </c>
-      <c r="Q85" s="73">
+      <c r="Q85" s="61">
         <v>0</v>
       </c>
-      <c r="R85" s="73">
+      <c r="R85" s="61">
         <v>0</v>
       </c>
-      <c r="S85" s="73">
+      <c r="S85" s="61">
         <v>0</v>
       </c>
-      <c r="T85" s="73">
+      <c r="T85" s="61">
         <v>0</v>
       </c>
-      <c r="U85" s="73">
+      <c r="U85" s="61">
         <v>0.79008697100000003</v>
       </c>
-      <c r="V85" s="73">
+      <c r="V85" s="61">
         <v>0</v>
       </c>
-      <c r="W85" s="74">
+      <c r="W85" s="62">
         <v>8.4400000000000005E-5</v>
       </c>
     </row>
     <row r="86" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A86" s="75">
+      <c r="A86" s="63">
         <v>3</v>
       </c>
-      <c r="B86" s="75">
+      <c r="B86" s="63">
         <v>38</v>
       </c>
-      <c r="C86" s="75">
+      <c r="C86" s="63">
         <v>25</v>
       </c>
-      <c r="D86" s="75">
+      <c r="D86" s="63">
         <v>29.722550179999999</v>
       </c>
-      <c r="E86" s="75">
+      <c r="E86" s="63">
         <v>0</v>
       </c>
-      <c r="F86" s="75">
+      <c r="F86" s="63">
         <v>1</v>
       </c>
-      <c r="G86" s="75">
+      <c r="G86" s="63">
         <v>1</v>
       </c>
-      <c r="H86" s="75">
+      <c r="H86" s="63">
         <v>1</v>
       </c>
-      <c r="I86" s="75">
+      <c r="I86" s="63">
         <v>20</v>
       </c>
-      <c r="J86" s="75">
+      <c r="J86" s="63">
         <v>8.26708E-4</v>
       </c>
-      <c r="K86" s="75">
+      <c r="K86" s="63">
         <v>1.4451199999999999E-4</v>
       </c>
-      <c r="L86" s="75">
+      <c r="L86" s="63">
         <v>0.16697783299999999</v>
       </c>
-      <c r="M86" s="75">
+      <c r="M86" s="63">
         <v>0</v>
       </c>
-      <c r="N86" s="76">
+      <c r="N86" s="64">
         <v>4.8099999999999997E-5</v>
       </c>
-      <c r="O86" s="75">
+      <c r="O86" s="63">
         <v>4.1753132999999998E-2</v>
       </c>
-      <c r="P86" s="75">
+      <c r="P86" s="63">
         <v>0</v>
       </c>
-      <c r="Q86" s="75">
+      <c r="Q86" s="63">
         <v>0</v>
       </c>
-      <c r="R86" s="75">
+      <c r="R86" s="63">
         <v>0</v>
       </c>
-      <c r="S86" s="75">
+      <c r="S86" s="63">
         <v>0</v>
       </c>
-      <c r="T86" s="75">
+      <c r="T86" s="63">
         <v>0</v>
       </c>
-      <c r="U86" s="75">
+      <c r="U86" s="63">
         <v>0.79011126899999995</v>
       </c>
-      <c r="V86" s="75">
+      <c r="V86" s="63">
         <v>0</v>
       </c>
-      <c r="W86" s="75">
+      <c r="W86" s="63">
         <v>1.383E-4</v>
       </c>
     </row>
     <row r="89" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A89" s="72" t="s">
+      <c r="A89" s="60" t="s">
         <v>461</v>
       </c>
-      <c r="B89" s="72" t="s">
+      <c r="B89" s="60" t="s">
         <v>484</v>
       </c>
-      <c r="C89" s="72" t="s">
+      <c r="C89" s="60" t="s">
         <v>485</v>
       </c>
-      <c r="D89" s="72">
+      <c r="D89" s="60">
         <v>4477696</v>
       </c>
-      <c r="E89" s="72">
+      <c r="E89" s="60">
         <v>4442130</v>
       </c>
-      <c r="F89" s="72">
+      <c r="F89" s="60">
         <v>4453535</v>
       </c>
-      <c r="G89" s="72">
+      <c r="G89" s="60">
         <v>4409545</v>
       </c>
-      <c r="H89" s="72">
+      <c r="H89" s="60">
         <v>4479989</v>
       </c>
-      <c r="I89" s="72">
+      <c r="I89" s="60">
         <v>4483174</v>
       </c>
-      <c r="J89" s="72">
+      <c r="J89" s="60">
         <v>4310398</v>
       </c>
-      <c r="K89" s="72">
+      <c r="K89" s="60">
         <v>4475758</v>
       </c>
-      <c r="L89" s="72">
+      <c r="L89" s="60">
         <v>4483015</v>
       </c>
-      <c r="M89" s="72">
+      <c r="M89" s="60">
         <v>1023075</v>
       </c>
-      <c r="N89" s="72">
+      <c r="N89" s="60">
         <v>4467992</v>
       </c>
-      <c r="O89" s="72">
+      <c r="O89" s="60">
         <v>4447416</v>
       </c>
-      <c r="P89" s="72">
+      <c r="P89" s="60">
         <v>4396235</v>
       </c>
-      <c r="Q89" s="72">
+      <c r="Q89" s="60">
         <v>4452538</v>
       </c>
-      <c r="R89" s="72">
+      <c r="R89" s="60">
         <v>4479603</v>
       </c>
-      <c r="S89" s="72">
+      <c r="S89" s="60">
         <v>4443574</v>
       </c>
-      <c r="T89" s="72">
+      <c r="T89" s="60">
         <v>1008348</v>
       </c>
-      <c r="U89" s="72">
+      <c r="U89" s="60">
         <v>4465803</v>
       </c>
-      <c r="V89" s="72">
+      <c r="V89" s="60">
         <v>1696853</v>
       </c>
       <c r="W89" s="25"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A90" s="73">
+      <c r="A90" s="61">
         <v>2</v>
       </c>
-      <c r="B90" s="73">
+      <c r="B90" s="61">
         <v>59</v>
       </c>
-      <c r="C90" s="73">
+      <c r="C90" s="61">
         <v>262</v>
       </c>
-      <c r="D90" s="73">
+      <c r="D90" s="61">
         <v>5.9274990000000001E-3</v>
       </c>
-      <c r="E90" s="73">
+      <c r="E90" s="61">
         <v>2.6355340000000001E-3</v>
       </c>
-      <c r="F90" s="73">
+      <c r="F90" s="61">
         <v>6.9169990000000001E-3</v>
       </c>
-      <c r="G90" s="73">
+      <c r="G90" s="61">
         <v>1.3904499999999999E-4</v>
       </c>
-      <c r="H90" s="73">
+      <c r="H90" s="61">
         <v>0.45107575999999999</v>
       </c>
-      <c r="I90" s="73">
+      <c r="I90" s="61">
         <v>0</v>
       </c>
-      <c r="J90" s="73">
+      <c r="J90" s="61">
         <v>1.17753E-4</v>
       </c>
-      <c r="K90" s="73">
+      <c r="K90" s="61">
         <v>0.20354787899999999</v>
       </c>
-      <c r="L90" s="73">
+      <c r="L90" s="61">
         <v>2.0555999999999999E-3</v>
       </c>
-      <c r="M90" s="73">
+      <c r="M90" s="61">
         <v>3.0082809999999998E-3</v>
       </c>
-      <c r="N90" s="73">
+      <c r="N90" s="61">
         <v>8.0592921999999997E-2</v>
       </c>
-      <c r="O90" s="74">
+      <c r="O90" s="62">
         <v>2.3799999999999999E-5</v>
       </c>
-      <c r="P90" s="73">
+      <c r="P90" s="61">
         <v>9.5061400000000002E-4</v>
       </c>
-      <c r="Q90" s="73">
+      <c r="Q90" s="61">
         <v>1.3842209999999999E-3</v>
       </c>
-      <c r="R90" s="73">
+      <c r="R90" s="61">
         <v>1.0308729000000001E-2</v>
       </c>
-      <c r="S90" s="73">
+      <c r="S90" s="61">
         <v>0</v>
       </c>
-      <c r="T90" s="73">
+      <c r="T90" s="61">
         <v>1.1927299999999999E-3</v>
       </c>
-      <c r="U90" s="73">
+      <c r="U90" s="61">
         <v>0</v>
       </c>
-      <c r="V90" s="73">
+      <c r="V90" s="61">
         <v>2.5571999999999999E-3</v>
       </c>
     </row>
     <row r="91" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A91" s="75">
+      <c r="A91" s="63">
         <v>2</v>
       </c>
-      <c r="B91" s="75">
+      <c r="B91" s="63">
         <v>73</v>
       </c>
-      <c r="C91" s="75">
+      <c r="C91" s="63">
         <v>262</v>
       </c>
-      <c r="D91" s="75">
+      <c r="D91" s="63">
         <v>1.6550118999999999E-2</v>
       </c>
-      <c r="E91" s="75">
+      <c r="E91" s="63">
         <v>6.086836E-3</v>
       </c>
-      <c r="F91" s="75">
+      <c r="F91" s="63">
         <v>9.0947560000000007E-3</v>
       </c>
-      <c r="G91" s="75">
+      <c r="G91" s="63">
         <v>2.49008E-4</v>
       </c>
-      <c r="H91" s="75">
+      <c r="H91" s="63">
         <v>0.50548730600000003</v>
       </c>
-      <c r="I91" s="75">
+      <c r="I91" s="63">
         <v>1.5042219999999999E-3</v>
       </c>
-      <c r="J91" s="75">
+      <c r="J91" s="63">
         <v>2.31208E-4</v>
       </c>
-      <c r="K91" s="75">
+      <c r="K91" s="63">
         <v>9.0964627000000006E-2</v>
       </c>
-      <c r="L91" s="75">
+      <c r="L91" s="63">
         <v>2.262525E-3</v>
       </c>
-      <c r="M91" s="75">
+      <c r="M91" s="63">
         <v>2.5396730000000001E-3</v>
       </c>
-      <c r="N91" s="75">
+      <c r="N91" s="63">
         <v>5.6683187000000003E-2</v>
       </c>
-      <c r="O91" s="75">
+      <c r="O91" s="63">
         <v>1.7504838000000002E-2</v>
       </c>
-      <c r="P91" s="75">
+      <c r="P91" s="63">
         <v>1.650966E-3</v>
       </c>
-      <c r="Q91" s="75">
+      <c r="Q91" s="63">
         <v>1.8998610000000001E-3</v>
       </c>
-      <c r="R91" s="75">
+      <c r="R91" s="63">
         <v>1.0040403E-2</v>
       </c>
-      <c r="S91" s="75">
+      <c r="S91" s="63">
         <v>6.8909519999999997E-3</v>
       </c>
-      <c r="T91" s="75">
+      <c r="T91" s="63">
         <v>1.0329390000000001E-3</v>
       </c>
-      <c r="U91" s="75">
+      <c r="U91" s="63">
         <v>0</v>
       </c>
-      <c r="V91" s="75">
+      <c r="V91" s="63">
         <v>3.7968110000000002E-3</v>
       </c>
     </row>
     <row r="92" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A92" s="73">
+      <c r="A92" s="61">
         <v>2</v>
       </c>
-      <c r="B92" s="73">
+      <c r="B92" s="61">
         <v>87</v>
       </c>
-      <c r="C92" s="73">
+      <c r="C92" s="61">
         <v>262</v>
       </c>
-      <c r="D92" s="73">
+      <c r="D92" s="61">
         <v>1.7835073999999999E-2</v>
       </c>
-      <c r="E92" s="73">
+      <c r="E92" s="61">
         <v>7.6499339999999997E-3</v>
       </c>
-      <c r="F92" s="73">
+      <c r="F92" s="61">
         <v>8.1510369999999999E-3</v>
       </c>
-      <c r="G92" s="73">
+      <c r="G92" s="61">
         <v>2.8239500000000001E-4</v>
       </c>
-      <c r="H92" s="73">
+      <c r="H92" s="61">
         <v>0.72203508599999999</v>
       </c>
-      <c r="I92" s="73">
+      <c r="I92" s="61">
         <v>7.7239199999999996E-3</v>
       </c>
-      <c r="J92" s="73">
+      <c r="J92" s="61">
         <v>2.9477399999999998E-4</v>
       </c>
-      <c r="K92" s="73">
+      <c r="K92" s="61">
         <v>6.1359282000000001E-2</v>
       </c>
-      <c r="L92" s="73">
+      <c r="L92" s="61">
         <v>1.4889910000000001E-3</v>
       </c>
-      <c r="M92" s="73">
+      <c r="M92" s="61">
         <v>1.0320419999999999E-3</v>
       </c>
-      <c r="N92" s="73">
+      <c r="N92" s="61">
         <v>3.2703910000000003E-2</v>
       </c>
-      <c r="O92" s="73">
+      <c r="O92" s="61">
         <v>0</v>
       </c>
-      <c r="P92" s="73">
+      <c r="P92" s="61">
         <v>1.6983549999999999E-3</v>
       </c>
-      <c r="Q92" s="73">
+      <c r="Q92" s="61">
         <v>1.883909E-3</v>
       </c>
-      <c r="R92" s="73">
+      <c r="R92" s="61">
         <v>6.6217469999999999E-3</v>
       </c>
-      <c r="S92" s="73">
+      <c r="S92" s="61">
         <v>2.1107900999999998E-2</v>
       </c>
-      <c r="T92" s="73">
+      <c r="T92" s="61">
         <v>4.2338E-4</v>
       </c>
-      <c r="U92" s="74">
+      <c r="U92" s="62">
         <v>7.9000000000000006E-6</v>
       </c>
-      <c r="V92" s="73">
+      <c r="V92" s="61">
         <v>3.8441080000000002E-3</v>
       </c>
     </row>
     <row r="93" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A93" s="75">
+      <c r="A93" s="63">
         <v>2</v>
       </c>
-      <c r="B93" s="75">
+      <c r="B93" s="63">
         <v>101</v>
       </c>
-      <c r="C93" s="75">
+      <c r="C93" s="63">
         <v>262</v>
       </c>
-      <c r="D93" s="75">
+      <c r="D93" s="63">
         <v>4.8287199999999999E-3</v>
       </c>
-      <c r="E93" s="75">
+      <c r="E93" s="63">
         <v>8.0598760000000005E-3</v>
       </c>
-      <c r="F93" s="75">
+      <c r="F93" s="63">
         <v>7.3449689999999998E-3</v>
       </c>
-      <c r="G93" s="75">
+      <c r="G93" s="63">
         <v>2.90406E-4</v>
       </c>
-      <c r="H93" s="75">
+      <c r="H93" s="63">
         <v>0.25782157900000002</v>
       </c>
-      <c r="I93" s="75">
+      <c r="I93" s="63">
         <v>3.8139850000000002E-3</v>
       </c>
-      <c r="J93" s="75">
+      <c r="J93" s="63">
         <v>3.41238E-4</v>
       </c>
-      <c r="K93" s="75">
+      <c r="K93" s="63">
         <v>1.80676E-2</v>
       </c>
-      <c r="L93" s="75">
+      <c r="L93" s="63">
         <v>8.3995300000000005E-4</v>
       </c>
-      <c r="M93" s="75">
+      <c r="M93" s="63">
         <v>1.5578099999999999E-4</v>
       </c>
-      <c r="N93" s="75">
+      <c r="N93" s="63">
         <v>2.293125E-3</v>
       </c>
-      <c r="O93" s="75">
+      <c r="O93" s="63">
         <v>6.8269299999999995E-4</v>
       </c>
-      <c r="P93" s="75">
+      <c r="P93" s="63">
         <v>1.499626E-3</v>
       </c>
-      <c r="Q93" s="75">
+      <c r="Q93" s="63">
         <v>1.7775149999999999E-3</v>
       </c>
-      <c r="R93" s="75">
+      <c r="R93" s="63">
         <v>3.7660279999999998E-3</v>
       </c>
-      <c r="S93" s="75">
+      <c r="S93" s="63">
         <v>1.610591E-3</v>
       </c>
-      <c r="T93" s="76">
+      <c r="T93" s="64">
         <v>1.2799999999999999E-5</v>
       </c>
-      <c r="U93" s="76">
+      <c r="U93" s="64">
         <v>1.34E-5</v>
       </c>
-      <c r="V93" s="75">
+      <c r="V93" s="63">
         <v>3.5811390000000001E-3</v>
       </c>
     </row>
@@ -13258,316 +13258,316 @@
       <c r="R94" s="25"/>
     </row>
     <row r="96" spans="1:26" ht="15.75" thickBot="1">
-      <c r="A96" s="72" t="s">
+      <c r="A96" s="60" t="s">
         <v>461</v>
       </c>
-      <c r="B96" s="72" t="s">
+      <c r="B96" s="60" t="s">
         <v>486</v>
       </c>
-      <c r="C96" s="72" t="s">
+      <c r="C96" s="60" t="s">
         <v>487</v>
       </c>
-      <c r="D96" s="72" t="s">
+      <c r="D96" s="60" t="s">
         <v>488</v>
       </c>
-      <c r="E96" s="72" t="s">
+      <c r="E96" s="60" t="s">
         <v>489</v>
       </c>
-      <c r="F96" s="72" t="s">
+      <c r="F96" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="G96" s="72" t="s">
+      <c r="G96" s="60" t="s">
         <v>491</v>
       </c>
-      <c r="H96" s="72" t="s">
+      <c r="H96" s="60" t="s">
         <v>492</v>
       </c>
-      <c r="I96" s="72" t="s">
+      <c r="I96" s="60" t="s">
         <v>493</v>
       </c>
-      <c r="J96" s="72" t="s">
+      <c r="J96" s="60" t="s">
         <v>494</v>
       </c>
-      <c r="K96" s="72" t="s">
+      <c r="K96" s="60" t="s">
         <v>495</v>
       </c>
-      <c r="L96" s="72" t="s">
+      <c r="L96" s="60" t="s">
         <v>496</v>
       </c>
-      <c r="M96" s="72" t="s">
+      <c r="M96" s="60" t="s">
         <v>497</v>
       </c>
-      <c r="N96" s="72" t="s">
+      <c r="N96" s="60" t="s">
         <v>498</v>
       </c>
-      <c r="O96" s="72" t="s">
+      <c r="O96" s="60" t="s">
         <v>499</v>
       </c>
-      <c r="P96" s="72" t="s">
+      <c r="P96" s="60" t="s">
         <v>500</v>
       </c>
-      <c r="Q96" s="72" t="s">
+      <c r="Q96" s="60" t="s">
         <v>501</v>
       </c>
-      <c r="R96" s="72" t="s">
+      <c r="R96" s="60" t="s">
         <v>502</v>
       </c>
-      <c r="S96" s="72" t="s">
+      <c r="S96" s="60" t="s">
         <v>503</v>
       </c>
-      <c r="T96" s="72" t="s">
+      <c r="T96" s="60" t="s">
         <v>504</v>
       </c>
-      <c r="U96" s="72" t="s">
+      <c r="U96" s="60" t="s">
         <v>505</v>
       </c>
-      <c r="V96" s="72" t="s">
+      <c r="V96" s="60" t="s">
         <v>506</v>
       </c>
-      <c r="W96" s="72" t="s">
+      <c r="W96" s="60" t="s">
         <v>507</v>
       </c>
-      <c r="X96" s="72" t="s">
+      <c r="X96" s="60" t="s">
         <v>508</v>
       </c>
-      <c r="Y96" s="72" t="s">
+      <c r="Y96" s="60" t="s">
         <v>509</v>
       </c>
       <c r="Z96" s="25"/>
     </row>
     <row r="97" spans="1:25" ht="15.75" thickBot="1">
-      <c r="A97" s="73">
+      <c r="A97" s="61">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B97" s="73">
+      <c r="B97" s="61">
         <v>0</v>
       </c>
-      <c r="C97" s="74">
+      <c r="C97" s="62">
         <v>4.0599999999999998E-5</v>
       </c>
-      <c r="D97" s="73">
+      <c r="D97" s="61">
         <v>1.946433E-3</v>
       </c>
-      <c r="E97" s="73">
+      <c r="E97" s="61">
         <v>0</v>
       </c>
-      <c r="F97" s="73">
+      <c r="F97" s="61">
         <v>1.0729822999999999E-2</v>
       </c>
-      <c r="G97" s="73">
+      <c r="G97" s="61">
         <v>4.1896541000000002E-2</v>
       </c>
-      <c r="H97" s="73">
+      <c r="H97" s="61">
         <v>7.7626300000000002E-4</v>
       </c>
-      <c r="I97" s="73">
+      <c r="I97" s="61">
         <v>0</v>
       </c>
-      <c r="J97" s="73">
+      <c r="J97" s="61">
         <v>5.1525599999999996E-4</v>
       </c>
-      <c r="K97" s="73">
+      <c r="K97" s="61">
         <v>0.49333814399999998</v>
       </c>
-      <c r="L97" s="73">
+      <c r="L97" s="61">
         <v>1.938111E-3</v>
       </c>
-      <c r="M97" s="73">
+      <c r="M97" s="61">
         <v>1.2953507E-2</v>
       </c>
-      <c r="N97" s="73">
+      <c r="N97" s="61">
         <v>5.0174400000000004E-4</v>
       </c>
-      <c r="O97" s="73">
+      <c r="O97" s="61">
         <v>9.0231939999999997E-2</v>
       </c>
-      <c r="P97" s="74">
+      <c r="P97" s="62">
         <v>9.2800000000000006E-5</v>
       </c>
-      <c r="Q97" s="73">
+      <c r="Q97" s="61">
         <v>2.9041174999999999E-2</v>
       </c>
-      <c r="R97" s="73">
+      <c r="R97" s="61">
         <v>6.7826639999999999E-3</v>
       </c>
-      <c r="S97" s="74">
+      <c r="S97" s="62">
         <v>7.3499999999999998E-5</v>
       </c>
-      <c r="T97" s="73">
+      <c r="T97" s="61">
         <v>0</v>
       </c>
-      <c r="U97" s="73">
+      <c r="U97" s="61">
         <v>2.242033E-3</v>
       </c>
-      <c r="V97" s="73">
+      <c r="V97" s="61">
         <v>1.7755119999999999E-3</v>
       </c>
-      <c r="W97" s="73">
+      <c r="W97" s="61">
         <v>4.9386229999999996E-3</v>
       </c>
-      <c r="X97" s="73">
+      <c r="X97" s="61">
         <v>5.8052799999999997E-4</v>
       </c>
-      <c r="Y97" s="73">
+      <c r="Y97" s="61">
         <v>3.4587442000000003E-2</v>
       </c>
     </row>
     <row r="98" spans="1:25" ht="15.75" thickBot="1">
-      <c r="A98" s="75">
+      <c r="A98" s="63">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B98" s="75">
+      <c r="B98" s="63">
         <v>14</v>
       </c>
-      <c r="C98" s="75">
+      <c r="C98" s="63">
         <v>1.562461E-3</v>
       </c>
-      <c r="D98" s="75">
+      <c r="D98" s="63">
         <v>1.2770030000000001E-3</v>
       </c>
-      <c r="E98" s="75">
+      <c r="E98" s="63">
         <v>6.4541299999999995E-4</v>
       </c>
-      <c r="F98" s="75">
+      <c r="F98" s="63">
         <v>7.2902349999999999E-3</v>
       </c>
-      <c r="G98" s="75">
+      <c r="G98" s="63">
         <v>0</v>
       </c>
-      <c r="H98" s="75">
+      <c r="H98" s="63">
         <v>4.7252399999999999E-4</v>
       </c>
-      <c r="I98" s="76">
+      <c r="I98" s="64">
         <v>3.7100000000000001E-5</v>
       </c>
-      <c r="J98" s="75">
+      <c r="J98" s="63">
         <v>2.9523800000000002E-4</v>
       </c>
-      <c r="K98" s="75">
+      <c r="K98" s="63">
         <v>0.71350525499999995</v>
       </c>
-      <c r="L98" s="75">
+      <c r="L98" s="63">
         <v>6.5623920000000002E-3</v>
       </c>
-      <c r="M98" s="75">
+      <c r="M98" s="63">
         <v>1.1915082E-2</v>
       </c>
-      <c r="N98" s="75">
+      <c r="N98" s="63">
         <v>3.0565399999999998E-4</v>
       </c>
-      <c r="O98" s="75">
+      <c r="O98" s="63">
         <v>2.9839318E-2</v>
       </c>
-      <c r="P98" s="76">
+      <c r="P98" s="64">
         <v>7.75E-5</v>
       </c>
-      <c r="Q98" s="75">
+      <c r="Q98" s="63">
         <v>2.0216921999999998E-2</v>
       </c>
-      <c r="R98" s="75">
+      <c r="R98" s="63">
         <v>4.4166819999999999E-3</v>
       </c>
-      <c r="S98" s="76">
+      <c r="S98" s="64">
         <v>8.0199999999999998E-5</v>
       </c>
-      <c r="T98" s="76">
+      <c r="T98" s="64">
         <v>2.5500000000000001E-6</v>
       </c>
-      <c r="U98" s="75">
+      <c r="U98" s="63">
         <v>1.7998529999999999E-3</v>
       </c>
-      <c r="V98" s="75">
+      <c r="V98" s="63">
         <v>1.516379E-3</v>
       </c>
-      <c r="W98" s="75">
+      <c r="W98" s="63">
         <v>2.8182569999999998E-3</v>
       </c>
-      <c r="X98" s="75">
+      <c r="X98" s="63">
         <v>3.5214000000000003E-4</v>
       </c>
-      <c r="Y98" s="75">
+      <c r="Y98" s="63">
         <v>1.8032133999999998E-2</v>
       </c>
     </row>
     <row r="99" spans="1:25" ht="15.75" thickBot="1">
-      <c r="A99" s="73">
+      <c r="A99" s="61">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B99" s="73">
+      <c r="B99" s="61">
         <v>28</v>
       </c>
-      <c r="C99" s="73">
+      <c r="C99" s="61">
         <v>3.5234820000000001E-3</v>
       </c>
-      <c r="D99" s="73">
+      <c r="D99" s="61">
         <v>1.5052799999999999E-3</v>
       </c>
-      <c r="E99" s="73">
+      <c r="E99" s="61">
         <v>1.8240649999999999E-3</v>
       </c>
-      <c r="F99" s="73">
+      <c r="F99" s="61">
         <v>8.8743980000000004E-3</v>
       </c>
-      <c r="G99" s="73">
+      <c r="G99" s="61">
         <v>2.1289333000000001E-2</v>
       </c>
-      <c r="H99" s="73">
+      <c r="H99" s="61">
         <v>5.1050900000000003E-4</v>
       </c>
-      <c r="I99" s="73">
+      <c r="I99" s="61">
         <v>1.02019E-4</v>
       </c>
-      <c r="J99" s="73">
+      <c r="J99" s="61">
         <v>2.95574E-4</v>
       </c>
-      <c r="K99" s="73">
+      <c r="K99" s="61">
         <v>0.65988184299999997</v>
       </c>
-      <c r="L99" s="73">
+      <c r="L99" s="61">
         <v>1.3712502999999999E-2</v>
       </c>
-      <c r="M99" s="73">
+      <c r="M99" s="61">
         <v>1.7759629999999998E-2</v>
       </c>
-      <c r="N99" s="73">
+      <c r="N99" s="61">
         <v>3.3933100000000001E-4</v>
       </c>
-      <c r="O99" s="73">
+      <c r="O99" s="61">
         <v>7.5271909999999999E-3</v>
       </c>
-      <c r="P99" s="73">
+      <c r="P99" s="61">
         <v>1.0993300000000001E-4</v>
       </c>
-      <c r="Q99" s="73">
+      <c r="Q99" s="61">
         <v>2.4865589E-2</v>
       </c>
-      <c r="R99" s="73">
+      <c r="R99" s="61">
         <v>5.1579620000000003E-3</v>
       </c>
-      <c r="S99" s="73">
+      <c r="S99" s="61">
         <v>1.29004E-4</v>
       </c>
-      <c r="T99" s="74">
+      <c r="T99" s="62">
         <v>8.1799999999999996E-6</v>
       </c>
-      <c r="U99" s="73">
+      <c r="U99" s="61">
         <v>2.513506E-3</v>
       </c>
-      <c r="V99" s="73">
+      <c r="V99" s="61">
         <v>2.1619460000000001E-3</v>
       </c>
-      <c r="W99" s="73">
+      <c r="W99" s="61">
         <v>2.8500489999999999E-3</v>
       </c>
-      <c r="X99" s="73">
+      <c r="X99" s="61">
         <v>3.79823E-4</v>
       </c>
-      <c r="Y99" s="73">
+      <c r="Y99" s="61">
         <v>1.7655562E-2</v>
       </c>
     </row>
     <row r="100" spans="1:25" ht="15.75" thickBot="1">
-      <c r="A100" s="75"/>
+      <c r="A100" s="63"/>
       <c r="B100" s="25"/>
       <c r="C100" s="25"/>
       <c r="D100" s="25"/>
@@ -13595,25 +13595,93 @@
     </row>
   </sheetData>
   <mergeCells count="130">
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="O47:R47"/>
-    <mergeCell ref="S47:V47"/>
-    <mergeCell ref="W47:Z47"/>
-    <mergeCell ref="AA47:AD47"/>
-    <mergeCell ref="AE47:AH47"/>
-    <mergeCell ref="AI47:AL47"/>
-    <mergeCell ref="AM47:AP47"/>
-    <mergeCell ref="BK47:BN47"/>
-    <mergeCell ref="BO47:BR47"/>
-    <mergeCell ref="BS47:BV47"/>
-    <mergeCell ref="BW47:BZ47"/>
-    <mergeCell ref="AQ47:AT47"/>
-    <mergeCell ref="AU47:AX47"/>
-    <mergeCell ref="AY47:BB47"/>
-    <mergeCell ref="BC47:BF47"/>
-    <mergeCell ref="BG47:BJ47"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="O8:S8"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="AX8:BB8"/>
+    <mergeCell ref="BC8:BG8"/>
+    <mergeCell ref="BH8:BL8"/>
+    <mergeCell ref="BM8:BQ8"/>
+    <mergeCell ref="BR8:BV8"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:X3"/>
+    <mergeCell ref="BW8:CA8"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="AD8:AH8"/>
+    <mergeCell ref="AI8:AM8"/>
+    <mergeCell ref="AN8:AR8"/>
+    <mergeCell ref="AS8:AW8"/>
+    <mergeCell ref="DF8:DJ8"/>
+    <mergeCell ref="DK8:DO8"/>
+    <mergeCell ref="DP8:DT8"/>
+    <mergeCell ref="DU8:DY8"/>
+    <mergeCell ref="DZ8:EE8"/>
+    <mergeCell ref="EF8:EK8"/>
+    <mergeCell ref="CB8:CF8"/>
+    <mergeCell ref="CG8:CK8"/>
+    <mergeCell ref="CL8:CP8"/>
+    <mergeCell ref="CQ8:CU8"/>
+    <mergeCell ref="CV8:CZ8"/>
+    <mergeCell ref="DA8:DE8"/>
+    <mergeCell ref="FV8:GA8"/>
+    <mergeCell ref="GB8:GG8"/>
+    <mergeCell ref="GH8:GM8"/>
+    <mergeCell ref="GN8:GS8"/>
+    <mergeCell ref="GT8:GY8"/>
+    <mergeCell ref="GZ8:HE8"/>
+    <mergeCell ref="EL8:EQ8"/>
+    <mergeCell ref="ER8:EW8"/>
+    <mergeCell ref="EX8:FC8"/>
+    <mergeCell ref="FD8:FI8"/>
+    <mergeCell ref="FJ8:FO8"/>
+    <mergeCell ref="FP8:FU8"/>
+    <mergeCell ref="IP8:IU8"/>
+    <mergeCell ref="IV8:JA8"/>
+    <mergeCell ref="JB8:JG8"/>
+    <mergeCell ref="JH8:JM8"/>
+    <mergeCell ref="JN8:JS8"/>
+    <mergeCell ref="JT8:JY8"/>
+    <mergeCell ref="HF8:HK8"/>
+    <mergeCell ref="HL8:HQ8"/>
+    <mergeCell ref="HR8:HW8"/>
+    <mergeCell ref="HX8:IC8"/>
+    <mergeCell ref="ID8:II8"/>
+    <mergeCell ref="IJ8:IO8"/>
+    <mergeCell ref="LP8:LU8"/>
+    <mergeCell ref="LV8:MA8"/>
+    <mergeCell ref="MB8:MG8"/>
+    <mergeCell ref="MH8:MM8"/>
+    <mergeCell ref="MN8:MS8"/>
+    <mergeCell ref="JZ8:KE8"/>
+    <mergeCell ref="KF8:KK8"/>
+    <mergeCell ref="KL8:KQ8"/>
+    <mergeCell ref="KR8:KW8"/>
+    <mergeCell ref="KX8:LC8"/>
+    <mergeCell ref="LD8:LI8"/>
     <mergeCell ref="QX8:RC8"/>
     <mergeCell ref="RD8:RI8"/>
     <mergeCell ref="RJ8:RO8"/>
@@ -13638,93 +13706,25 @@
     <mergeCell ref="NR8:NW8"/>
     <mergeCell ref="NX8:OC8"/>
     <mergeCell ref="LJ8:LO8"/>
-    <mergeCell ref="LP8:LU8"/>
-    <mergeCell ref="LV8:MA8"/>
-    <mergeCell ref="MB8:MG8"/>
-    <mergeCell ref="MH8:MM8"/>
-    <mergeCell ref="MN8:MS8"/>
-    <mergeCell ref="JZ8:KE8"/>
-    <mergeCell ref="KF8:KK8"/>
-    <mergeCell ref="KL8:KQ8"/>
-    <mergeCell ref="KR8:KW8"/>
-    <mergeCell ref="KX8:LC8"/>
-    <mergeCell ref="LD8:LI8"/>
-    <mergeCell ref="IP8:IU8"/>
-    <mergeCell ref="IV8:JA8"/>
-    <mergeCell ref="JB8:JG8"/>
-    <mergeCell ref="JH8:JM8"/>
-    <mergeCell ref="JN8:JS8"/>
-    <mergeCell ref="JT8:JY8"/>
-    <mergeCell ref="HF8:HK8"/>
-    <mergeCell ref="HL8:HQ8"/>
-    <mergeCell ref="HR8:HW8"/>
-    <mergeCell ref="HX8:IC8"/>
-    <mergeCell ref="ID8:II8"/>
-    <mergeCell ref="IJ8:IO8"/>
-    <mergeCell ref="FV8:GA8"/>
-    <mergeCell ref="GB8:GG8"/>
-    <mergeCell ref="GH8:GM8"/>
-    <mergeCell ref="GN8:GS8"/>
-    <mergeCell ref="GT8:GY8"/>
-    <mergeCell ref="GZ8:HE8"/>
-    <mergeCell ref="EL8:EQ8"/>
-    <mergeCell ref="ER8:EW8"/>
-    <mergeCell ref="EX8:FC8"/>
-    <mergeCell ref="FD8:FI8"/>
-    <mergeCell ref="FJ8:FO8"/>
-    <mergeCell ref="FP8:FU8"/>
-    <mergeCell ref="DP8:DT8"/>
-    <mergeCell ref="DU8:DY8"/>
-    <mergeCell ref="DZ8:EE8"/>
-    <mergeCell ref="EF8:EK8"/>
-    <mergeCell ref="CB8:CF8"/>
-    <mergeCell ref="CG8:CK8"/>
-    <mergeCell ref="CL8:CP8"/>
-    <mergeCell ref="CQ8:CU8"/>
-    <mergeCell ref="CV8:CZ8"/>
-    <mergeCell ref="DA8:DE8"/>
-    <mergeCell ref="BW8:CA8"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="AD8:AH8"/>
-    <mergeCell ref="AI8:AM8"/>
-    <mergeCell ref="AN8:AR8"/>
-    <mergeCell ref="AS8:AW8"/>
-    <mergeCell ref="DF8:DJ8"/>
-    <mergeCell ref="DK8:DO8"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="AX8:BB8"/>
-    <mergeCell ref="BC8:BG8"/>
-    <mergeCell ref="BH8:BL8"/>
-    <mergeCell ref="BM8:BQ8"/>
-    <mergeCell ref="BR8:BV8"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:X3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="O8:S8"/>
-    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="AM47:AP47"/>
+    <mergeCell ref="BK47:BN47"/>
+    <mergeCell ref="BO47:BR47"/>
+    <mergeCell ref="BS47:BV47"/>
+    <mergeCell ref="BW47:BZ47"/>
+    <mergeCell ref="AQ47:AT47"/>
+    <mergeCell ref="AU47:AX47"/>
+    <mergeCell ref="AY47:BB47"/>
+    <mergeCell ref="BC47:BF47"/>
+    <mergeCell ref="BG47:BJ47"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="O47:R47"/>
+    <mergeCell ref="S47:V47"/>
+    <mergeCell ref="W47:Z47"/>
+    <mergeCell ref="AA47:AD47"/>
+    <mergeCell ref="AE47:AH47"/>
+    <mergeCell ref="AI47:AL47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A16" r:id="rId1" xr:uid="{3202BA62-C7C1-44C7-931A-B83B37570BA9}"/>
@@ -14292,69 +14292,69 @@
       </c>
     </row>
     <row r="40" spans="5:13">
-      <c r="E40" s="60" t="s">
+      <c r="E40" s="65" t="s">
         <v>377</v>
       </c>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="60"/>
-      <c r="J40" s="60"/>
-      <c r="K40" s="60"/>
-      <c r="L40" s="60"/>
-      <c r="M40" s="60"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="65"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="65"/>
+      <c r="M40" s="65"/>
     </row>
     <row r="41" spans="5:13">
-      <c r="E41" s="61" t="s">
+      <c r="E41" s="66" t="s">
         <v>378</v>
       </c>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="61"/>
-      <c r="K41" s="61"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="61"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="66"/>
+      <c r="K41" s="66"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="66"/>
     </row>
     <row r="42" spans="5:13">
-      <c r="E42" s="61" t="s">
+      <c r="E42" s="66" t="s">
         <v>379</v>
       </c>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="61"/>
-      <c r="J42" s="61"/>
-      <c r="K42" s="61"/>
-      <c r="L42" s="61"/>
-      <c r="M42" s="61"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="66"/>
+      <c r="J42" s="66"/>
+      <c r="K42" s="66"/>
+      <c r="L42" s="66"/>
+      <c r="M42" s="66"/>
     </row>
     <row r="43" spans="5:13">
-      <c r="E43" s="61" t="s">
+      <c r="E43" s="66" t="s">
         <v>380</v>
       </c>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="61"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="61"/>
-      <c r="L43" s="61"/>
-      <c r="M43" s="61"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
     </row>
     <row r="44" spans="5:13">
-      <c r="E44" s="61" t="s">
+      <c r="E44" s="66" t="s">
         <v>381</v>
       </c>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="61"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="61"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
     </row>
     <row r="47" spans="5:13">
       <c r="E47" t="s">
@@ -14645,7 +14645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58470E99-39F3-4288-B960-9BFE3E917FBC}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>

</xml_diff>